<commit_message>
scrum backlog updated for sprint3
</commit_message>
<xml_diff>
--- a/ch.bfh.bti7081.s2013.yellow/doc/cs1_task10/product_scrum_backlog.xlsx
+++ b/ch.bfh.bti7081.s2013.yellow/doc/cs1_task10/product_scrum_backlog.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\school\yellow\ch.bfh.bti7081.s2013.yellow\doc\cs1_task10\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -230,6 +230,18 @@
   </si>
   <si>
     <t>Installationsanleitung</t>
+  </si>
+  <si>
+    <t>glisb1 noch Apassungen machen</t>
+  </si>
+  <si>
+    <t>rohdj1/polla2</t>
+  </si>
+  <si>
+    <t>bronc1/glisb1</t>
+  </si>
+  <si>
+    <t>Implement Unit Tests</t>
   </si>
 </sst>
 </file>
@@ -478,7 +490,7 @@
     </a:clrScheme>
     <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -513,7 +525,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -724,23 +736,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.7109375"/>
-    <col min="2" max="2" width="24.5703125"/>
-    <col min="3" max="3" width="31.5703125"/>
-    <col min="4" max="4" width="7.28515625"/>
-    <col min="5" max="5" width="11.85546875"/>
-    <col min="6" max="6" width="13.28515625"/>
-    <col min="7" max="7" width="10.28515625"/>
-    <col min="8" max="8" width="14.5703125"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="60" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -789,7 +791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="14.5" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
@@ -812,7 +814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="14.5" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -838,7 +840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -864,6 +866,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -871,27 +878,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="4"/>
-    <col min="2" max="2" width="7" style="4"/>
-    <col min="3" max="3" width="25.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="28" style="6"/>
-    <col min="6" max="6" width="15.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="5"/>
-    <col min="8" max="8" width="9.5703125" style="5"/>
-    <col min="9" max="9" width="10.85546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="5"/>
-    <col min="11" max="11" width="17" style="5"/>
-    <col min="12" max="1025" width="9.140625" style="5"/>
+    <col min="1" max="2" width="9.1640625" style="4"/>
+    <col min="3" max="3" width="25.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="6"/>
+    <col min="6" max="6" width="15.5" style="5" customWidth="1"/>
+    <col min="7" max="8" width="9.1640625" style="5"/>
+    <col min="9" max="9" width="10.83203125" style="5" customWidth="1"/>
+    <col min="10" max="1025" width="9.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1025" s="8" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -926,7 +929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1025" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1025" ht="60" customHeight="1">
       <c r="A2" s="14">
         <v>3.4</v>
       </c>
@@ -1973,7 +1976,7 @@
       <c r="AMJ2" s="15"/>
       <c r="AMK2" s="15"/>
     </row>
-    <row r="3" spans="1:1025" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1025" ht="105" customHeight="1">
       <c r="A3" s="14">
         <v>3.7</v>
       </c>
@@ -3020,7 +3023,7 @@
       <c r="AMJ3" s="15"/>
       <c r="AMK3" s="15"/>
     </row>
-    <row r="4" spans="1:1025" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1025" ht="90" customHeight="1">
       <c r="A4" s="14">
         <v>3.1</v>
       </c>
@@ -4065,7 +4068,7 @@
       <c r="AMJ4" s="15"/>
       <c r="AMK4" s="15"/>
     </row>
-    <row r="5" spans="1:1025" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1025" s="17" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="14">
         <v>3.13</v>
       </c>
@@ -5112,7 +5115,7 @@
       <c r="AMJ5" s="15"/>
       <c r="AMK5" s="15"/>
     </row>
-    <row r="6" spans="1:1025" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1025" ht="45" customHeight="1">
       <c r="A6" s="14">
         <v>3.14</v>
       </c>
@@ -6159,7 +6162,7 @@
       <c r="AMJ6" s="15"/>
       <c r="AMK6" s="15"/>
     </row>
-    <row r="7" spans="1:1025" s="21" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1025" s="21" customFormat="1" ht="42">
       <c r="A7" s="18">
         <v>3.1</v>
       </c>
@@ -7202,7 +7205,7 @@
       <c r="AMJ7" s="19"/>
       <c r="AMK7" s="19"/>
     </row>
-    <row r="8" spans="1:1025" s="13" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1025" s="13" customFormat="1" ht="56">
       <c r="A8" s="10">
         <v>3.2</v>
       </c>
@@ -7228,7 +7231,9 @@
         <v>10</v>
       </c>
       <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="J8" s="11">
+        <v>7</v>
+      </c>
       <c r="K8" s="11" t="s">
         <v>12</v>
       </c>
@@ -8247,57 +8252,69 @@
       <c r="AMJ8" s="11"/>
       <c r="AMK8" s="11"/>
     </row>
-    <row r="9" spans="1:1025" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+    <row r="9" spans="1:1025" ht="70">
+      <c r="A9" s="10">
         <v>3.3</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="10">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="11">
         <v>16</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:1025" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="10" spans="1:1025" s="13" customFormat="1" ht="28">
+      <c r="A10" s="10">
         <v>3.5</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5" t="s">
+      <c r="H10" s="11">
+        <v>8</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="11"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
@@ -9312,7 +9329,7 @@
       <c r="AMJ10" s="5"/>
       <c r="AMK10" s="5"/>
     </row>
-    <row r="11" spans="1:1025" s="17" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1025" s="17" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="4">
         <v>3.6</v>
       </c>
@@ -10351,7 +10368,7 @@
       <c r="AMJ11" s="5"/>
       <c r="AMK11" s="5"/>
     </row>
-    <row r="12" spans="1:1025" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1025" ht="30" customHeight="1">
       <c r="A12" s="4">
         <v>3.8</v>
       </c>
@@ -10368,1054 +10385,39 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1025" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+    <row r="13" spans="1:1025" s="15" customFormat="1">
+      <c r="A13" s="14">
         <v>3.9</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="15">
         <v>2</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="15">
         <v>8</v>
       </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11">
+      <c r="J13" s="15">
         <v>7</v>
       </c>
-      <c r="K13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11"/>
-      <c r="AK13" s="11"/>
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="11"/>
-      <c r="AN13" s="11"/>
-      <c r="AO13" s="11"/>
-      <c r="AP13" s="11"/>
-      <c r="AQ13" s="11"/>
-      <c r="AR13" s="11"/>
-      <c r="AS13" s="11"/>
-      <c r="AT13" s="11"/>
-      <c r="AU13" s="11"/>
-      <c r="AV13" s="11"/>
-      <c r="AW13" s="11"/>
-      <c r="AX13" s="11"/>
-      <c r="AY13" s="11"/>
-      <c r="AZ13" s="11"/>
-      <c r="BA13" s="11"/>
-      <c r="BB13" s="11"/>
-      <c r="BC13" s="11"/>
-      <c r="BD13" s="11"/>
-      <c r="BE13" s="11"/>
-      <c r="BF13" s="11"/>
-      <c r="BG13" s="11"/>
-      <c r="BH13" s="11"/>
-      <c r="BI13" s="11"/>
-      <c r="BJ13" s="11"/>
-      <c r="BK13" s="11"/>
-      <c r="BL13" s="11"/>
-      <c r="BM13" s="11"/>
-      <c r="BN13" s="11"/>
-      <c r="BO13" s="11"/>
-      <c r="BP13" s="11"/>
-      <c r="BQ13" s="11"/>
-      <c r="BR13" s="11"/>
-      <c r="BS13" s="11"/>
-      <c r="BT13" s="11"/>
-      <c r="BU13" s="11"/>
-      <c r="BV13" s="11"/>
-      <c r="BW13" s="11"/>
-      <c r="BX13" s="11"/>
-      <c r="BY13" s="11"/>
-      <c r="BZ13" s="11"/>
-      <c r="CA13" s="11"/>
-      <c r="CB13" s="11"/>
-      <c r="CC13" s="11"/>
-      <c r="CD13" s="11"/>
-      <c r="CE13" s="11"/>
-      <c r="CF13" s="11"/>
-      <c r="CG13" s="11"/>
-      <c r="CH13" s="11"/>
-      <c r="CI13" s="11"/>
-      <c r="CJ13" s="11"/>
-      <c r="CK13" s="11"/>
-      <c r="CL13" s="11"/>
-      <c r="CM13" s="11"/>
-      <c r="CN13" s="11"/>
-      <c r="CO13" s="11"/>
-      <c r="CP13" s="11"/>
-      <c r="CQ13" s="11"/>
-      <c r="CR13" s="11"/>
-      <c r="CS13" s="11"/>
-      <c r="CT13" s="11"/>
-      <c r="CU13" s="11"/>
-      <c r="CV13" s="11"/>
-      <c r="CW13" s="11"/>
-      <c r="CX13" s="11"/>
-      <c r="CY13" s="11"/>
-      <c r="CZ13" s="11"/>
-      <c r="DA13" s="11"/>
-      <c r="DB13" s="11"/>
-      <c r="DC13" s="11"/>
-      <c r="DD13" s="11"/>
-      <c r="DE13" s="11"/>
-      <c r="DF13" s="11"/>
-      <c r="DG13" s="11"/>
-      <c r="DH13" s="11"/>
-      <c r="DI13" s="11"/>
-      <c r="DJ13" s="11"/>
-      <c r="DK13" s="11"/>
-      <c r="DL13" s="11"/>
-      <c r="DM13" s="11"/>
-      <c r="DN13" s="11"/>
-      <c r="DO13" s="11"/>
-      <c r="DP13" s="11"/>
-      <c r="DQ13" s="11"/>
-      <c r="DR13" s="11"/>
-      <c r="DS13" s="11"/>
-      <c r="DT13" s="11"/>
-      <c r="DU13" s="11"/>
-      <c r="DV13" s="11"/>
-      <c r="DW13" s="11"/>
-      <c r="DX13" s="11"/>
-      <c r="DY13" s="11"/>
-      <c r="DZ13" s="11"/>
-      <c r="EA13" s="11"/>
-      <c r="EB13" s="11"/>
-      <c r="EC13" s="11"/>
-      <c r="ED13" s="11"/>
-      <c r="EE13" s="11"/>
-      <c r="EF13" s="11"/>
-      <c r="EG13" s="11"/>
-      <c r="EH13" s="11"/>
-      <c r="EI13" s="11"/>
-      <c r="EJ13" s="11"/>
-      <c r="EK13" s="11"/>
-      <c r="EL13" s="11"/>
-      <c r="EM13" s="11"/>
-      <c r="EN13" s="11"/>
-      <c r="EO13" s="11"/>
-      <c r="EP13" s="11"/>
-      <c r="EQ13" s="11"/>
-      <c r="ER13" s="11"/>
-      <c r="ES13" s="11"/>
-      <c r="ET13" s="11"/>
-      <c r="EU13" s="11"/>
-      <c r="EV13" s="11"/>
-      <c r="EW13" s="11"/>
-      <c r="EX13" s="11"/>
-      <c r="EY13" s="11"/>
-      <c r="EZ13" s="11"/>
-      <c r="FA13" s="11"/>
-      <c r="FB13" s="11"/>
-      <c r="FC13" s="11"/>
-      <c r="FD13" s="11"/>
-      <c r="FE13" s="11"/>
-      <c r="FF13" s="11"/>
-      <c r="FG13" s="11"/>
-      <c r="FH13" s="11"/>
-      <c r="FI13" s="11"/>
-      <c r="FJ13" s="11"/>
-      <c r="FK13" s="11"/>
-      <c r="FL13" s="11"/>
-      <c r="FM13" s="11"/>
-      <c r="FN13" s="11"/>
-      <c r="FO13" s="11"/>
-      <c r="FP13" s="11"/>
-      <c r="FQ13" s="11"/>
-      <c r="FR13" s="11"/>
-      <c r="FS13" s="11"/>
-      <c r="FT13" s="11"/>
-      <c r="FU13" s="11"/>
-      <c r="FV13" s="11"/>
-      <c r="FW13" s="11"/>
-      <c r="FX13" s="11"/>
-      <c r="FY13" s="11"/>
-      <c r="FZ13" s="11"/>
-      <c r="GA13" s="11"/>
-      <c r="GB13" s="11"/>
-      <c r="GC13" s="11"/>
-      <c r="GD13" s="11"/>
-      <c r="GE13" s="11"/>
-      <c r="GF13" s="11"/>
-      <c r="GG13" s="11"/>
-      <c r="GH13" s="11"/>
-      <c r="GI13" s="11"/>
-      <c r="GJ13" s="11"/>
-      <c r="GK13" s="11"/>
-      <c r="GL13" s="11"/>
-      <c r="GM13" s="11"/>
-      <c r="GN13" s="11"/>
-      <c r="GO13" s="11"/>
-      <c r="GP13" s="11"/>
-      <c r="GQ13" s="11"/>
-      <c r="GR13" s="11"/>
-      <c r="GS13" s="11"/>
-      <c r="GT13" s="11"/>
-      <c r="GU13" s="11"/>
-      <c r="GV13" s="11"/>
-      <c r="GW13" s="11"/>
-      <c r="GX13" s="11"/>
-      <c r="GY13" s="11"/>
-      <c r="GZ13" s="11"/>
-      <c r="HA13" s="11"/>
-      <c r="HB13" s="11"/>
-      <c r="HC13" s="11"/>
-      <c r="HD13" s="11"/>
-      <c r="HE13" s="11"/>
-      <c r="HF13" s="11"/>
-      <c r="HG13" s="11"/>
-      <c r="HH13" s="11"/>
-      <c r="HI13" s="11"/>
-      <c r="HJ13" s="11"/>
-      <c r="HK13" s="11"/>
-      <c r="HL13" s="11"/>
-      <c r="HM13" s="11"/>
-      <c r="HN13" s="11"/>
-      <c r="HO13" s="11"/>
-      <c r="HP13" s="11"/>
-      <c r="HQ13" s="11"/>
-      <c r="HR13" s="11"/>
-      <c r="HS13" s="11"/>
-      <c r="HT13" s="11"/>
-      <c r="HU13" s="11"/>
-      <c r="HV13" s="11"/>
-      <c r="HW13" s="11"/>
-      <c r="HX13" s="11"/>
-      <c r="HY13" s="11"/>
-      <c r="HZ13" s="11"/>
-      <c r="IA13" s="11"/>
-      <c r="IB13" s="11"/>
-      <c r="IC13" s="11"/>
-      <c r="ID13" s="11"/>
-      <c r="IE13" s="11"/>
-      <c r="IF13" s="11"/>
-      <c r="IG13" s="11"/>
-      <c r="IH13" s="11"/>
-      <c r="II13" s="11"/>
-      <c r="IJ13" s="11"/>
-      <c r="IK13" s="11"/>
-      <c r="IL13" s="11"/>
-      <c r="IM13" s="11"/>
-      <c r="IN13" s="11"/>
-      <c r="IO13" s="11"/>
-      <c r="IP13" s="11"/>
-      <c r="IQ13" s="11"/>
-      <c r="IR13" s="11"/>
-      <c r="IS13" s="11"/>
-      <c r="IT13" s="11"/>
-      <c r="IU13" s="11"/>
-      <c r="IV13" s="11"/>
-      <c r="IW13" s="11"/>
-      <c r="IX13" s="11"/>
-      <c r="IY13" s="11"/>
-      <c r="IZ13" s="11"/>
-      <c r="JA13" s="11"/>
-      <c r="JB13" s="11"/>
-      <c r="JC13" s="11"/>
-      <c r="JD13" s="11"/>
-      <c r="JE13" s="11"/>
-      <c r="JF13" s="11"/>
-      <c r="JG13" s="11"/>
-      <c r="JH13" s="11"/>
-      <c r="JI13" s="11"/>
-      <c r="JJ13" s="11"/>
-      <c r="JK13" s="11"/>
-      <c r="JL13" s="11"/>
-      <c r="JM13" s="11"/>
-      <c r="JN13" s="11"/>
-      <c r="JO13" s="11"/>
-      <c r="JP13" s="11"/>
-      <c r="JQ13" s="11"/>
-      <c r="JR13" s="11"/>
-      <c r="JS13" s="11"/>
-      <c r="JT13" s="11"/>
-      <c r="JU13" s="11"/>
-      <c r="JV13" s="11"/>
-      <c r="JW13" s="11"/>
-      <c r="JX13" s="11"/>
-      <c r="JY13" s="11"/>
-      <c r="JZ13" s="11"/>
-      <c r="KA13" s="11"/>
-      <c r="KB13" s="11"/>
-      <c r="KC13" s="11"/>
-      <c r="KD13" s="11"/>
-      <c r="KE13" s="11"/>
-      <c r="KF13" s="11"/>
-      <c r="KG13" s="11"/>
-      <c r="KH13" s="11"/>
-      <c r="KI13" s="11"/>
-      <c r="KJ13" s="11"/>
-      <c r="KK13" s="11"/>
-      <c r="KL13" s="11"/>
-      <c r="KM13" s="11"/>
-      <c r="KN13" s="11"/>
-      <c r="KO13" s="11"/>
-      <c r="KP13" s="11"/>
-      <c r="KQ13" s="11"/>
-      <c r="KR13" s="11"/>
-      <c r="KS13" s="11"/>
-      <c r="KT13" s="11"/>
-      <c r="KU13" s="11"/>
-      <c r="KV13" s="11"/>
-      <c r="KW13" s="11"/>
-      <c r="KX13" s="11"/>
-      <c r="KY13" s="11"/>
-      <c r="KZ13" s="11"/>
-      <c r="LA13" s="11"/>
-      <c r="LB13" s="11"/>
-      <c r="LC13" s="11"/>
-      <c r="LD13" s="11"/>
-      <c r="LE13" s="11"/>
-      <c r="LF13" s="11"/>
-      <c r="LG13" s="11"/>
-      <c r="LH13" s="11"/>
-      <c r="LI13" s="11"/>
-      <c r="LJ13" s="11"/>
-      <c r="LK13" s="11"/>
-      <c r="LL13" s="11"/>
-      <c r="LM13" s="11"/>
-      <c r="LN13" s="11"/>
-      <c r="LO13" s="11"/>
-      <c r="LP13" s="11"/>
-      <c r="LQ13" s="11"/>
-      <c r="LR13" s="11"/>
-      <c r="LS13" s="11"/>
-      <c r="LT13" s="11"/>
-      <c r="LU13" s="11"/>
-      <c r="LV13" s="11"/>
-      <c r="LW13" s="11"/>
-      <c r="LX13" s="11"/>
-      <c r="LY13" s="11"/>
-      <c r="LZ13" s="11"/>
-      <c r="MA13" s="11"/>
-      <c r="MB13" s="11"/>
-      <c r="MC13" s="11"/>
-      <c r="MD13" s="11"/>
-      <c r="ME13" s="11"/>
-      <c r="MF13" s="11"/>
-      <c r="MG13" s="11"/>
-      <c r="MH13" s="11"/>
-      <c r="MI13" s="11"/>
-      <c r="MJ13" s="11"/>
-      <c r="MK13" s="11"/>
-      <c r="ML13" s="11"/>
-      <c r="MM13" s="11"/>
-      <c r="MN13" s="11"/>
-      <c r="MO13" s="11"/>
-      <c r="MP13" s="11"/>
-      <c r="MQ13" s="11"/>
-      <c r="MR13" s="11"/>
-      <c r="MS13" s="11"/>
-      <c r="MT13" s="11"/>
-      <c r="MU13" s="11"/>
-      <c r="MV13" s="11"/>
-      <c r="MW13" s="11"/>
-      <c r="MX13" s="11"/>
-      <c r="MY13" s="11"/>
-      <c r="MZ13" s="11"/>
-      <c r="NA13" s="11"/>
-      <c r="NB13" s="11"/>
-      <c r="NC13" s="11"/>
-      <c r="ND13" s="11"/>
-      <c r="NE13" s="11"/>
-      <c r="NF13" s="11"/>
-      <c r="NG13" s="11"/>
-      <c r="NH13" s="11"/>
-      <c r="NI13" s="11"/>
-      <c r="NJ13" s="11"/>
-      <c r="NK13" s="11"/>
-      <c r="NL13" s="11"/>
-      <c r="NM13" s="11"/>
-      <c r="NN13" s="11"/>
-      <c r="NO13" s="11"/>
-      <c r="NP13" s="11"/>
-      <c r="NQ13" s="11"/>
-      <c r="NR13" s="11"/>
-      <c r="NS13" s="11"/>
-      <c r="NT13" s="11"/>
-      <c r="NU13" s="11"/>
-      <c r="NV13" s="11"/>
-      <c r="NW13" s="11"/>
-      <c r="NX13" s="11"/>
-      <c r="NY13" s="11"/>
-      <c r="NZ13" s="11"/>
-      <c r="OA13" s="11"/>
-      <c r="OB13" s="11"/>
-      <c r="OC13" s="11"/>
-      <c r="OD13" s="11"/>
-      <c r="OE13" s="11"/>
-      <c r="OF13" s="11"/>
-      <c r="OG13" s="11"/>
-      <c r="OH13" s="11"/>
-      <c r="OI13" s="11"/>
-      <c r="OJ13" s="11"/>
-      <c r="OK13" s="11"/>
-      <c r="OL13" s="11"/>
-      <c r="OM13" s="11"/>
-      <c r="ON13" s="11"/>
-      <c r="OO13" s="11"/>
-      <c r="OP13" s="11"/>
-      <c r="OQ13" s="11"/>
-      <c r="OR13" s="11"/>
-      <c r="OS13" s="11"/>
-      <c r="OT13" s="11"/>
-      <c r="OU13" s="11"/>
-      <c r="OV13" s="11"/>
-      <c r="OW13" s="11"/>
-      <c r="OX13" s="11"/>
-      <c r="OY13" s="11"/>
-      <c r="OZ13" s="11"/>
-      <c r="PA13" s="11"/>
-      <c r="PB13" s="11"/>
-      <c r="PC13" s="11"/>
-      <c r="PD13" s="11"/>
-      <c r="PE13" s="11"/>
-      <c r="PF13" s="11"/>
-      <c r="PG13" s="11"/>
-      <c r="PH13" s="11"/>
-      <c r="PI13" s="11"/>
-      <c r="PJ13" s="11"/>
-      <c r="PK13" s="11"/>
-      <c r="PL13" s="11"/>
-      <c r="PM13" s="11"/>
-      <c r="PN13" s="11"/>
-      <c r="PO13" s="11"/>
-      <c r="PP13" s="11"/>
-      <c r="PQ13" s="11"/>
-      <c r="PR13" s="11"/>
-      <c r="PS13" s="11"/>
-      <c r="PT13" s="11"/>
-      <c r="PU13" s="11"/>
-      <c r="PV13" s="11"/>
-      <c r="PW13" s="11"/>
-      <c r="PX13" s="11"/>
-      <c r="PY13" s="11"/>
-      <c r="PZ13" s="11"/>
-      <c r="QA13" s="11"/>
-      <c r="QB13" s="11"/>
-      <c r="QC13" s="11"/>
-      <c r="QD13" s="11"/>
-      <c r="QE13" s="11"/>
-      <c r="QF13" s="11"/>
-      <c r="QG13" s="11"/>
-      <c r="QH13" s="11"/>
-      <c r="QI13" s="11"/>
-      <c r="QJ13" s="11"/>
-      <c r="QK13" s="11"/>
-      <c r="QL13" s="11"/>
-      <c r="QM13" s="11"/>
-      <c r="QN13" s="11"/>
-      <c r="QO13" s="11"/>
-      <c r="QP13" s="11"/>
-      <c r="QQ13" s="11"/>
-      <c r="QR13" s="11"/>
-      <c r="QS13" s="11"/>
-      <c r="QT13" s="11"/>
-      <c r="QU13" s="11"/>
-      <c r="QV13" s="11"/>
-      <c r="QW13" s="11"/>
-      <c r="QX13" s="11"/>
-      <c r="QY13" s="11"/>
-      <c r="QZ13" s="11"/>
-      <c r="RA13" s="11"/>
-      <c r="RB13" s="11"/>
-      <c r="RC13" s="11"/>
-      <c r="RD13" s="11"/>
-      <c r="RE13" s="11"/>
-      <c r="RF13" s="11"/>
-      <c r="RG13" s="11"/>
-      <c r="RH13" s="11"/>
-      <c r="RI13" s="11"/>
-      <c r="RJ13" s="11"/>
-      <c r="RK13" s="11"/>
-      <c r="RL13" s="11"/>
-      <c r="RM13" s="11"/>
-      <c r="RN13" s="11"/>
-      <c r="RO13" s="11"/>
-      <c r="RP13" s="11"/>
-      <c r="RQ13" s="11"/>
-      <c r="RR13" s="11"/>
-      <c r="RS13" s="11"/>
-      <c r="RT13" s="11"/>
-      <c r="RU13" s="11"/>
-      <c r="RV13" s="11"/>
-      <c r="RW13" s="11"/>
-      <c r="RX13" s="11"/>
-      <c r="RY13" s="11"/>
-      <c r="RZ13" s="11"/>
-      <c r="SA13" s="11"/>
-      <c r="SB13" s="11"/>
-      <c r="SC13" s="11"/>
-      <c r="SD13" s="11"/>
-      <c r="SE13" s="11"/>
-      <c r="SF13" s="11"/>
-      <c r="SG13" s="11"/>
-      <c r="SH13" s="11"/>
-      <c r="SI13" s="11"/>
-      <c r="SJ13" s="11"/>
-      <c r="SK13" s="11"/>
-      <c r="SL13" s="11"/>
-      <c r="SM13" s="11"/>
-      <c r="SN13" s="11"/>
-      <c r="SO13" s="11"/>
-      <c r="SP13" s="11"/>
-      <c r="SQ13" s="11"/>
-      <c r="SR13" s="11"/>
-      <c r="SS13" s="11"/>
-      <c r="ST13" s="11"/>
-      <c r="SU13" s="11"/>
-      <c r="SV13" s="11"/>
-      <c r="SW13" s="11"/>
-      <c r="SX13" s="11"/>
-      <c r="SY13" s="11"/>
-      <c r="SZ13" s="11"/>
-      <c r="TA13" s="11"/>
-      <c r="TB13" s="11"/>
-      <c r="TC13" s="11"/>
-      <c r="TD13" s="11"/>
-      <c r="TE13" s="11"/>
-      <c r="TF13" s="11"/>
-      <c r="TG13" s="11"/>
-      <c r="TH13" s="11"/>
-      <c r="TI13" s="11"/>
-      <c r="TJ13" s="11"/>
-      <c r="TK13" s="11"/>
-      <c r="TL13" s="11"/>
-      <c r="TM13" s="11"/>
-      <c r="TN13" s="11"/>
-      <c r="TO13" s="11"/>
-      <c r="TP13" s="11"/>
-      <c r="TQ13" s="11"/>
-      <c r="TR13" s="11"/>
-      <c r="TS13" s="11"/>
-      <c r="TT13" s="11"/>
-      <c r="TU13" s="11"/>
-      <c r="TV13" s="11"/>
-      <c r="TW13" s="11"/>
-      <c r="TX13" s="11"/>
-      <c r="TY13" s="11"/>
-      <c r="TZ13" s="11"/>
-      <c r="UA13" s="11"/>
-      <c r="UB13" s="11"/>
-      <c r="UC13" s="11"/>
-      <c r="UD13" s="11"/>
-      <c r="UE13" s="11"/>
-      <c r="UF13" s="11"/>
-      <c r="UG13" s="11"/>
-      <c r="UH13" s="11"/>
-      <c r="UI13" s="11"/>
-      <c r="UJ13" s="11"/>
-      <c r="UK13" s="11"/>
-      <c r="UL13" s="11"/>
-      <c r="UM13" s="11"/>
-      <c r="UN13" s="11"/>
-      <c r="UO13" s="11"/>
-      <c r="UP13" s="11"/>
-      <c r="UQ13" s="11"/>
-      <c r="UR13" s="11"/>
-      <c r="US13" s="11"/>
-      <c r="UT13" s="11"/>
-      <c r="UU13" s="11"/>
-      <c r="UV13" s="11"/>
-      <c r="UW13" s="11"/>
-      <c r="UX13" s="11"/>
-      <c r="UY13" s="11"/>
-      <c r="UZ13" s="11"/>
-      <c r="VA13" s="11"/>
-      <c r="VB13" s="11"/>
-      <c r="VC13" s="11"/>
-      <c r="VD13" s="11"/>
-      <c r="VE13" s="11"/>
-      <c r="VF13" s="11"/>
-      <c r="VG13" s="11"/>
-      <c r="VH13" s="11"/>
-      <c r="VI13" s="11"/>
-      <c r="VJ13" s="11"/>
-      <c r="VK13" s="11"/>
-      <c r="VL13" s="11"/>
-      <c r="VM13" s="11"/>
-      <c r="VN13" s="11"/>
-      <c r="VO13" s="11"/>
-      <c r="VP13" s="11"/>
-      <c r="VQ13" s="11"/>
-      <c r="VR13" s="11"/>
-      <c r="VS13" s="11"/>
-      <c r="VT13" s="11"/>
-      <c r="VU13" s="11"/>
-      <c r="VV13" s="11"/>
-      <c r="VW13" s="11"/>
-      <c r="VX13" s="11"/>
-      <c r="VY13" s="11"/>
-      <c r="VZ13" s="11"/>
-      <c r="WA13" s="11"/>
-      <c r="WB13" s="11"/>
-      <c r="WC13" s="11"/>
-      <c r="WD13" s="11"/>
-      <c r="WE13" s="11"/>
-      <c r="WF13" s="11"/>
-      <c r="WG13" s="11"/>
-      <c r="WH13" s="11"/>
-      <c r="WI13" s="11"/>
-      <c r="WJ13" s="11"/>
-      <c r="WK13" s="11"/>
-      <c r="WL13" s="11"/>
-      <c r="WM13" s="11"/>
-      <c r="WN13" s="11"/>
-      <c r="WO13" s="11"/>
-      <c r="WP13" s="11"/>
-      <c r="WQ13" s="11"/>
-      <c r="WR13" s="11"/>
-      <c r="WS13" s="11"/>
-      <c r="WT13" s="11"/>
-      <c r="WU13" s="11"/>
-      <c r="WV13" s="11"/>
-      <c r="WW13" s="11"/>
-      <c r="WX13" s="11"/>
-      <c r="WY13" s="11"/>
-      <c r="WZ13" s="11"/>
-      <c r="XA13" s="11"/>
-      <c r="XB13" s="11"/>
-      <c r="XC13" s="11"/>
-      <c r="XD13" s="11"/>
-      <c r="XE13" s="11"/>
-      <c r="XF13" s="11"/>
-      <c r="XG13" s="11"/>
-      <c r="XH13" s="11"/>
-      <c r="XI13" s="11"/>
-      <c r="XJ13" s="11"/>
-      <c r="XK13" s="11"/>
-      <c r="XL13" s="11"/>
-      <c r="XM13" s="11"/>
-      <c r="XN13" s="11"/>
-      <c r="XO13" s="11"/>
-      <c r="XP13" s="11"/>
-      <c r="XQ13" s="11"/>
-      <c r="XR13" s="11"/>
-      <c r="XS13" s="11"/>
-      <c r="XT13" s="11"/>
-      <c r="XU13" s="11"/>
-      <c r="XV13" s="11"/>
-      <c r="XW13" s="11"/>
-      <c r="XX13" s="11"/>
-      <c r="XY13" s="11"/>
-      <c r="XZ13" s="11"/>
-      <c r="YA13" s="11"/>
-      <c r="YB13" s="11"/>
-      <c r="YC13" s="11"/>
-      <c r="YD13" s="11"/>
-      <c r="YE13" s="11"/>
-      <c r="YF13" s="11"/>
-      <c r="YG13" s="11"/>
-      <c r="YH13" s="11"/>
-      <c r="YI13" s="11"/>
-      <c r="YJ13" s="11"/>
-      <c r="YK13" s="11"/>
-      <c r="YL13" s="11"/>
-      <c r="YM13" s="11"/>
-      <c r="YN13" s="11"/>
-      <c r="YO13" s="11"/>
-      <c r="YP13" s="11"/>
-      <c r="YQ13" s="11"/>
-      <c r="YR13" s="11"/>
-      <c r="YS13" s="11"/>
-      <c r="YT13" s="11"/>
-      <c r="YU13" s="11"/>
-      <c r="YV13" s="11"/>
-      <c r="YW13" s="11"/>
-      <c r="YX13" s="11"/>
-      <c r="YY13" s="11"/>
-      <c r="YZ13" s="11"/>
-      <c r="ZA13" s="11"/>
-      <c r="ZB13" s="11"/>
-      <c r="ZC13" s="11"/>
-      <c r="ZD13" s="11"/>
-      <c r="ZE13" s="11"/>
-      <c r="ZF13" s="11"/>
-      <c r="ZG13" s="11"/>
-      <c r="ZH13" s="11"/>
-      <c r="ZI13" s="11"/>
-      <c r="ZJ13" s="11"/>
-      <c r="ZK13" s="11"/>
-      <c r="ZL13" s="11"/>
-      <c r="ZM13" s="11"/>
-      <c r="ZN13" s="11"/>
-      <c r="ZO13" s="11"/>
-      <c r="ZP13" s="11"/>
-      <c r="ZQ13" s="11"/>
-      <c r="ZR13" s="11"/>
-      <c r="ZS13" s="11"/>
-      <c r="ZT13" s="11"/>
-      <c r="ZU13" s="11"/>
-      <c r="ZV13" s="11"/>
-      <c r="ZW13" s="11"/>
-      <c r="ZX13" s="11"/>
-      <c r="ZY13" s="11"/>
-      <c r="ZZ13" s="11"/>
-      <c r="AAA13" s="11"/>
-      <c r="AAB13" s="11"/>
-      <c r="AAC13" s="11"/>
-      <c r="AAD13" s="11"/>
-      <c r="AAE13" s="11"/>
-      <c r="AAF13" s="11"/>
-      <c r="AAG13" s="11"/>
-      <c r="AAH13" s="11"/>
-      <c r="AAI13" s="11"/>
-      <c r="AAJ13" s="11"/>
-      <c r="AAK13" s="11"/>
-      <c r="AAL13" s="11"/>
-      <c r="AAM13" s="11"/>
-      <c r="AAN13" s="11"/>
-      <c r="AAO13" s="11"/>
-      <c r="AAP13" s="11"/>
-      <c r="AAQ13" s="11"/>
-      <c r="AAR13" s="11"/>
-      <c r="AAS13" s="11"/>
-      <c r="AAT13" s="11"/>
-      <c r="AAU13" s="11"/>
-      <c r="AAV13" s="11"/>
-      <c r="AAW13" s="11"/>
-      <c r="AAX13" s="11"/>
-      <c r="AAY13" s="11"/>
-      <c r="AAZ13" s="11"/>
-      <c r="ABA13" s="11"/>
-      <c r="ABB13" s="11"/>
-      <c r="ABC13" s="11"/>
-      <c r="ABD13" s="11"/>
-      <c r="ABE13" s="11"/>
-      <c r="ABF13" s="11"/>
-      <c r="ABG13" s="11"/>
-      <c r="ABH13" s="11"/>
-      <c r="ABI13" s="11"/>
-      <c r="ABJ13" s="11"/>
-      <c r="ABK13" s="11"/>
-      <c r="ABL13" s="11"/>
-      <c r="ABM13" s="11"/>
-      <c r="ABN13" s="11"/>
-      <c r="ABO13" s="11"/>
-      <c r="ABP13" s="11"/>
-      <c r="ABQ13" s="11"/>
-      <c r="ABR13" s="11"/>
-      <c r="ABS13" s="11"/>
-      <c r="ABT13" s="11"/>
-      <c r="ABU13" s="11"/>
-      <c r="ABV13" s="11"/>
-      <c r="ABW13" s="11"/>
-      <c r="ABX13" s="11"/>
-      <c r="ABY13" s="11"/>
-      <c r="ABZ13" s="11"/>
-      <c r="ACA13" s="11"/>
-      <c r="ACB13" s="11"/>
-      <c r="ACC13" s="11"/>
-      <c r="ACD13" s="11"/>
-      <c r="ACE13" s="11"/>
-      <c r="ACF13" s="11"/>
-      <c r="ACG13" s="11"/>
-      <c r="ACH13" s="11"/>
-      <c r="ACI13" s="11"/>
-      <c r="ACJ13" s="11"/>
-      <c r="ACK13" s="11"/>
-      <c r="ACL13" s="11"/>
-      <c r="ACM13" s="11"/>
-      <c r="ACN13" s="11"/>
-      <c r="ACO13" s="11"/>
-      <c r="ACP13" s="11"/>
-      <c r="ACQ13" s="11"/>
-      <c r="ACR13" s="11"/>
-      <c r="ACS13" s="11"/>
-      <c r="ACT13" s="11"/>
-      <c r="ACU13" s="11"/>
-      <c r="ACV13" s="11"/>
-      <c r="ACW13" s="11"/>
-      <c r="ACX13" s="11"/>
-      <c r="ACY13" s="11"/>
-      <c r="ACZ13" s="11"/>
-      <c r="ADA13" s="11"/>
-      <c r="ADB13" s="11"/>
-      <c r="ADC13" s="11"/>
-      <c r="ADD13" s="11"/>
-      <c r="ADE13" s="11"/>
-      <c r="ADF13" s="11"/>
-      <c r="ADG13" s="11"/>
-      <c r="ADH13" s="11"/>
-      <c r="ADI13" s="11"/>
-      <c r="ADJ13" s="11"/>
-      <c r="ADK13" s="11"/>
-      <c r="ADL13" s="11"/>
-      <c r="ADM13" s="11"/>
-      <c r="ADN13" s="11"/>
-      <c r="ADO13" s="11"/>
-      <c r="ADP13" s="11"/>
-      <c r="ADQ13" s="11"/>
-      <c r="ADR13" s="11"/>
-      <c r="ADS13" s="11"/>
-      <c r="ADT13" s="11"/>
-      <c r="ADU13" s="11"/>
-      <c r="ADV13" s="11"/>
-      <c r="ADW13" s="11"/>
-      <c r="ADX13" s="11"/>
-      <c r="ADY13" s="11"/>
-      <c r="ADZ13" s="11"/>
-      <c r="AEA13" s="11"/>
-      <c r="AEB13" s="11"/>
-      <c r="AEC13" s="11"/>
-      <c r="AED13" s="11"/>
-      <c r="AEE13" s="11"/>
-      <c r="AEF13" s="11"/>
-      <c r="AEG13" s="11"/>
-      <c r="AEH13" s="11"/>
-      <c r="AEI13" s="11"/>
-      <c r="AEJ13" s="11"/>
-      <c r="AEK13" s="11"/>
-      <c r="AEL13" s="11"/>
-      <c r="AEM13" s="11"/>
-      <c r="AEN13" s="11"/>
-      <c r="AEO13" s="11"/>
-      <c r="AEP13" s="11"/>
-      <c r="AEQ13" s="11"/>
-      <c r="AER13" s="11"/>
-      <c r="AES13" s="11"/>
-      <c r="AET13" s="11"/>
-      <c r="AEU13" s="11"/>
-      <c r="AEV13" s="11"/>
-      <c r="AEW13" s="11"/>
-      <c r="AEX13" s="11"/>
-      <c r="AEY13" s="11"/>
-      <c r="AEZ13" s="11"/>
-      <c r="AFA13" s="11"/>
-      <c r="AFB13" s="11"/>
-      <c r="AFC13" s="11"/>
-      <c r="AFD13" s="11"/>
-      <c r="AFE13" s="11"/>
-      <c r="AFF13" s="11"/>
-      <c r="AFG13" s="11"/>
-      <c r="AFH13" s="11"/>
-      <c r="AFI13" s="11"/>
-      <c r="AFJ13" s="11"/>
-      <c r="AFK13" s="11"/>
-      <c r="AFL13" s="11"/>
-      <c r="AFM13" s="11"/>
-      <c r="AFN13" s="11"/>
-      <c r="AFO13" s="11"/>
-      <c r="AFP13" s="11"/>
-      <c r="AFQ13" s="11"/>
-      <c r="AFR13" s="11"/>
-      <c r="AFS13" s="11"/>
-      <c r="AFT13" s="11"/>
-      <c r="AFU13" s="11"/>
-      <c r="AFV13" s="11"/>
-      <c r="AFW13" s="11"/>
-      <c r="AFX13" s="11"/>
-      <c r="AFY13" s="11"/>
-      <c r="AFZ13" s="11"/>
-      <c r="AGA13" s="11"/>
-      <c r="AGB13" s="11"/>
-      <c r="AGC13" s="11"/>
-      <c r="AGD13" s="11"/>
-      <c r="AGE13" s="11"/>
-      <c r="AGF13" s="11"/>
-      <c r="AGG13" s="11"/>
-      <c r="AGH13" s="11"/>
-      <c r="AGI13" s="11"/>
-      <c r="AGJ13" s="11"/>
-      <c r="AGK13" s="11"/>
-      <c r="AGL13" s="11"/>
-      <c r="AGM13" s="11"/>
-      <c r="AGN13" s="11"/>
-      <c r="AGO13" s="11"/>
-      <c r="AGP13" s="11"/>
-      <c r="AGQ13" s="11"/>
-      <c r="AGR13" s="11"/>
-      <c r="AGS13" s="11"/>
-      <c r="AGT13" s="11"/>
-      <c r="AGU13" s="11"/>
-      <c r="AGV13" s="11"/>
-      <c r="AGW13" s="11"/>
-      <c r="AGX13" s="11"/>
-      <c r="AGY13" s="11"/>
-      <c r="AGZ13" s="11"/>
-      <c r="AHA13" s="11"/>
-      <c r="AHB13" s="11"/>
-      <c r="AHC13" s="11"/>
-      <c r="AHD13" s="11"/>
-      <c r="AHE13" s="11"/>
-      <c r="AHF13" s="11"/>
-      <c r="AHG13" s="11"/>
-      <c r="AHH13" s="11"/>
-      <c r="AHI13" s="11"/>
-      <c r="AHJ13" s="11"/>
-      <c r="AHK13" s="11"/>
-      <c r="AHL13" s="11"/>
-      <c r="AHM13" s="11"/>
-      <c r="AHN13" s="11"/>
-      <c r="AHO13" s="11"/>
-      <c r="AHP13" s="11"/>
-      <c r="AHQ13" s="11"/>
-      <c r="AHR13" s="11"/>
-      <c r="AHS13" s="11"/>
-      <c r="AHT13" s="11"/>
-      <c r="AHU13" s="11"/>
-      <c r="AHV13" s="11"/>
-      <c r="AHW13" s="11"/>
-      <c r="AHX13" s="11"/>
-      <c r="AHY13" s="11"/>
-      <c r="AHZ13" s="11"/>
-      <c r="AIA13" s="11"/>
-      <c r="AIB13" s="11"/>
-      <c r="AIC13" s="11"/>
-      <c r="AID13" s="11"/>
-      <c r="AIE13" s="11"/>
-      <c r="AIF13" s="11"/>
-      <c r="AIG13" s="11"/>
-      <c r="AIH13" s="11"/>
-      <c r="AII13" s="11"/>
-      <c r="AIJ13" s="11"/>
-      <c r="AIK13" s="11"/>
-      <c r="AIL13" s="11"/>
-      <c r="AIM13" s="11"/>
-      <c r="AIN13" s="11"/>
-      <c r="AIO13" s="11"/>
-      <c r="AIP13" s="11"/>
-      <c r="AIQ13" s="11"/>
-      <c r="AIR13" s="11"/>
-      <c r="AIS13" s="11"/>
-      <c r="AIT13" s="11"/>
-      <c r="AIU13" s="11"/>
-      <c r="AIV13" s="11"/>
-      <c r="AIW13" s="11"/>
-      <c r="AIX13" s="11"/>
-      <c r="AIY13" s="11"/>
-      <c r="AIZ13" s="11"/>
-      <c r="AJA13" s="11"/>
-      <c r="AJB13" s="11"/>
-      <c r="AJC13" s="11"/>
-      <c r="AJD13" s="11"/>
-      <c r="AJE13" s="11"/>
-      <c r="AJF13" s="11"/>
-      <c r="AJG13" s="11"/>
-      <c r="AJH13" s="11"/>
-      <c r="AJI13" s="11"/>
-      <c r="AJJ13" s="11"/>
-      <c r="AJK13" s="11"/>
-      <c r="AJL13" s="11"/>
-      <c r="AJM13" s="11"/>
-      <c r="AJN13" s="11"/>
-      <c r="AJO13" s="11"/>
-      <c r="AJP13" s="11"/>
-      <c r="AJQ13" s="11"/>
-      <c r="AJR13" s="11"/>
-      <c r="AJS13" s="11"/>
-      <c r="AJT13" s="11"/>
-      <c r="AJU13" s="11"/>
-      <c r="AJV13" s="11"/>
-      <c r="AJW13" s="11"/>
-      <c r="AJX13" s="11"/>
-      <c r="AJY13" s="11"/>
-      <c r="AJZ13" s="11"/>
-      <c r="AKA13" s="11"/>
-      <c r="AKB13" s="11"/>
-      <c r="AKC13" s="11"/>
-      <c r="AKD13" s="11"/>
-      <c r="AKE13" s="11"/>
-      <c r="AKF13" s="11"/>
-      <c r="AKG13" s="11"/>
-      <c r="AKH13" s="11"/>
-      <c r="AKI13" s="11"/>
-      <c r="AKJ13" s="11"/>
-      <c r="AKK13" s="11"/>
-      <c r="AKL13" s="11"/>
-      <c r="AKM13" s="11"/>
-      <c r="AKN13" s="11"/>
-      <c r="AKO13" s="11"/>
-      <c r="AKP13" s="11"/>
-      <c r="AKQ13" s="11"/>
-      <c r="AKR13" s="11"/>
-      <c r="AKS13" s="11"/>
-      <c r="AKT13" s="11"/>
-      <c r="AKU13" s="11"/>
-      <c r="AKV13" s="11"/>
-      <c r="AKW13" s="11"/>
-      <c r="AKX13" s="11"/>
-      <c r="AKY13" s="11"/>
-      <c r="AKZ13" s="11"/>
-      <c r="ALA13" s="11"/>
-      <c r="ALB13" s="11"/>
-      <c r="ALC13" s="11"/>
-      <c r="ALD13" s="11"/>
-      <c r="ALE13" s="11"/>
-      <c r="ALF13" s="11"/>
-      <c r="ALG13" s="11"/>
-      <c r="ALH13" s="11"/>
-      <c r="ALI13" s="11"/>
-      <c r="ALJ13" s="11"/>
-      <c r="ALK13" s="11"/>
-      <c r="ALL13" s="11"/>
-      <c r="ALM13" s="11"/>
-      <c r="ALN13" s="11"/>
-      <c r="ALO13" s="11"/>
-      <c r="ALP13" s="11"/>
-      <c r="ALQ13" s="11"/>
-      <c r="ALR13" s="11"/>
-      <c r="ALS13" s="11"/>
-      <c r="ALT13" s="11"/>
-      <c r="ALU13" s="11"/>
-      <c r="ALV13" s="11"/>
-      <c r="ALW13" s="11"/>
-      <c r="ALX13" s="11"/>
-      <c r="ALY13" s="11"/>
-      <c r="ALZ13" s="11"/>
-      <c r="AMA13" s="11"/>
-      <c r="AMB13" s="11"/>
-      <c r="AMC13" s="11"/>
-      <c r="AMD13" s="11"/>
-      <c r="AME13" s="11"/>
-      <c r="AMF13" s="11"/>
-      <c r="AMG13" s="11"/>
-      <c r="AMH13" s="11"/>
-      <c r="AMI13" s="11"/>
-      <c r="AMJ13" s="11"/>
-      <c r="AMK13" s="11"/>
+      <c r="K13" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="14" spans="1:1025" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1025" s="17" customFormat="1" ht="28">
       <c r="A14" s="4">
         <v>3.11</v>
       </c>
@@ -12452,7 +11454,7 @@
       <c r="AMJ14" s="5"/>
       <c r="AMK14" s="5"/>
     </row>
-    <row r="15" spans="1:1025" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1025" s="13" customFormat="1" ht="28">
       <c r="A15" s="10">
         <v>3.16</v>
       </c>
@@ -12476,7 +11478,9 @@
         <v>6</v>
       </c>
       <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="J15" s="11">
+        <v>8</v>
+      </c>
       <c r="K15" s="11" t="s">
         <v>12</v>
       </c>
@@ -13495,1052 +12499,39 @@
       <c r="AMJ15" s="11"/>
       <c r="AMK15" s="11"/>
     </row>
-    <row r="16" spans="1:1025" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+    <row r="16" spans="1:1025" s="15" customFormat="1">
+      <c r="A16" s="14">
         <v>3.15</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="15">
         <v>2</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="15">
         <v>4</v>
       </c>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
-      <c r="AI16" s="11"/>
-      <c r="AJ16" s="11"/>
-      <c r="AK16" s="11"/>
-      <c r="AL16" s="11"/>
-      <c r="AM16" s="11"/>
-      <c r="AN16" s="11"/>
-      <c r="AO16" s="11"/>
-      <c r="AP16" s="11"/>
-      <c r="AQ16" s="11"/>
-      <c r="AR16" s="11"/>
-      <c r="AS16" s="11"/>
-      <c r="AT16" s="11"/>
-      <c r="AU16" s="11"/>
-      <c r="AV16" s="11"/>
-      <c r="AW16" s="11"/>
-      <c r="AX16" s="11"/>
-      <c r="AY16" s="11"/>
-      <c r="AZ16" s="11"/>
-      <c r="BA16" s="11"/>
-      <c r="BB16" s="11"/>
-      <c r="BC16" s="11"/>
-      <c r="BD16" s="11"/>
-      <c r="BE16" s="11"/>
-      <c r="BF16" s="11"/>
-      <c r="BG16" s="11"/>
-      <c r="BH16" s="11"/>
-      <c r="BI16" s="11"/>
-      <c r="BJ16" s="11"/>
-      <c r="BK16" s="11"/>
-      <c r="BL16" s="11"/>
-      <c r="BM16" s="11"/>
-      <c r="BN16" s="11"/>
-      <c r="BO16" s="11"/>
-      <c r="BP16" s="11"/>
-      <c r="BQ16" s="11"/>
-      <c r="BR16" s="11"/>
-      <c r="BS16" s="11"/>
-      <c r="BT16" s="11"/>
-      <c r="BU16" s="11"/>
-      <c r="BV16" s="11"/>
-      <c r="BW16" s="11"/>
-      <c r="BX16" s="11"/>
-      <c r="BY16" s="11"/>
-      <c r="BZ16" s="11"/>
-      <c r="CA16" s="11"/>
-      <c r="CB16" s="11"/>
-      <c r="CC16" s="11"/>
-      <c r="CD16" s="11"/>
-      <c r="CE16" s="11"/>
-      <c r="CF16" s="11"/>
-      <c r="CG16" s="11"/>
-      <c r="CH16" s="11"/>
-      <c r="CI16" s="11"/>
-      <c r="CJ16" s="11"/>
-      <c r="CK16" s="11"/>
-      <c r="CL16" s="11"/>
-      <c r="CM16" s="11"/>
-      <c r="CN16" s="11"/>
-      <c r="CO16" s="11"/>
-      <c r="CP16" s="11"/>
-      <c r="CQ16" s="11"/>
-      <c r="CR16" s="11"/>
-      <c r="CS16" s="11"/>
-      <c r="CT16" s="11"/>
-      <c r="CU16" s="11"/>
-      <c r="CV16" s="11"/>
-      <c r="CW16" s="11"/>
-      <c r="CX16" s="11"/>
-      <c r="CY16" s="11"/>
-      <c r="CZ16" s="11"/>
-      <c r="DA16" s="11"/>
-      <c r="DB16" s="11"/>
-      <c r="DC16" s="11"/>
-      <c r="DD16" s="11"/>
-      <c r="DE16" s="11"/>
-      <c r="DF16" s="11"/>
-      <c r="DG16" s="11"/>
-      <c r="DH16" s="11"/>
-      <c r="DI16" s="11"/>
-      <c r="DJ16" s="11"/>
-      <c r="DK16" s="11"/>
-      <c r="DL16" s="11"/>
-      <c r="DM16" s="11"/>
-      <c r="DN16" s="11"/>
-      <c r="DO16" s="11"/>
-      <c r="DP16" s="11"/>
-      <c r="DQ16" s="11"/>
-      <c r="DR16" s="11"/>
-      <c r="DS16" s="11"/>
-      <c r="DT16" s="11"/>
-      <c r="DU16" s="11"/>
-      <c r="DV16" s="11"/>
-      <c r="DW16" s="11"/>
-      <c r="DX16" s="11"/>
-      <c r="DY16" s="11"/>
-      <c r="DZ16" s="11"/>
-      <c r="EA16" s="11"/>
-      <c r="EB16" s="11"/>
-      <c r="EC16" s="11"/>
-      <c r="ED16" s="11"/>
-      <c r="EE16" s="11"/>
-      <c r="EF16" s="11"/>
-      <c r="EG16" s="11"/>
-      <c r="EH16" s="11"/>
-      <c r="EI16" s="11"/>
-      <c r="EJ16" s="11"/>
-      <c r="EK16" s="11"/>
-      <c r="EL16" s="11"/>
-      <c r="EM16" s="11"/>
-      <c r="EN16" s="11"/>
-      <c r="EO16" s="11"/>
-      <c r="EP16" s="11"/>
-      <c r="EQ16" s="11"/>
-      <c r="ER16" s="11"/>
-      <c r="ES16" s="11"/>
-      <c r="ET16" s="11"/>
-      <c r="EU16" s="11"/>
-      <c r="EV16" s="11"/>
-      <c r="EW16" s="11"/>
-      <c r="EX16" s="11"/>
-      <c r="EY16" s="11"/>
-      <c r="EZ16" s="11"/>
-      <c r="FA16" s="11"/>
-      <c r="FB16" s="11"/>
-      <c r="FC16" s="11"/>
-      <c r="FD16" s="11"/>
-      <c r="FE16" s="11"/>
-      <c r="FF16" s="11"/>
-      <c r="FG16" s="11"/>
-      <c r="FH16" s="11"/>
-      <c r="FI16" s="11"/>
-      <c r="FJ16" s="11"/>
-      <c r="FK16" s="11"/>
-      <c r="FL16" s="11"/>
-      <c r="FM16" s="11"/>
-      <c r="FN16" s="11"/>
-      <c r="FO16" s="11"/>
-      <c r="FP16" s="11"/>
-      <c r="FQ16" s="11"/>
-      <c r="FR16" s="11"/>
-      <c r="FS16" s="11"/>
-      <c r="FT16" s="11"/>
-      <c r="FU16" s="11"/>
-      <c r="FV16" s="11"/>
-      <c r="FW16" s="11"/>
-      <c r="FX16" s="11"/>
-      <c r="FY16" s="11"/>
-      <c r="FZ16" s="11"/>
-      <c r="GA16" s="11"/>
-      <c r="GB16" s="11"/>
-      <c r="GC16" s="11"/>
-      <c r="GD16" s="11"/>
-      <c r="GE16" s="11"/>
-      <c r="GF16" s="11"/>
-      <c r="GG16" s="11"/>
-      <c r="GH16" s="11"/>
-      <c r="GI16" s="11"/>
-      <c r="GJ16" s="11"/>
-      <c r="GK16" s="11"/>
-      <c r="GL16" s="11"/>
-      <c r="GM16" s="11"/>
-      <c r="GN16" s="11"/>
-      <c r="GO16" s="11"/>
-      <c r="GP16" s="11"/>
-      <c r="GQ16" s="11"/>
-      <c r="GR16" s="11"/>
-      <c r="GS16" s="11"/>
-      <c r="GT16" s="11"/>
-      <c r="GU16" s="11"/>
-      <c r="GV16" s="11"/>
-      <c r="GW16" s="11"/>
-      <c r="GX16" s="11"/>
-      <c r="GY16" s="11"/>
-      <c r="GZ16" s="11"/>
-      <c r="HA16" s="11"/>
-      <c r="HB16" s="11"/>
-      <c r="HC16" s="11"/>
-      <c r="HD16" s="11"/>
-      <c r="HE16" s="11"/>
-      <c r="HF16" s="11"/>
-      <c r="HG16" s="11"/>
-      <c r="HH16" s="11"/>
-      <c r="HI16" s="11"/>
-      <c r="HJ16" s="11"/>
-      <c r="HK16" s="11"/>
-      <c r="HL16" s="11"/>
-      <c r="HM16" s="11"/>
-      <c r="HN16" s="11"/>
-      <c r="HO16" s="11"/>
-      <c r="HP16" s="11"/>
-      <c r="HQ16" s="11"/>
-      <c r="HR16" s="11"/>
-      <c r="HS16" s="11"/>
-      <c r="HT16" s="11"/>
-      <c r="HU16" s="11"/>
-      <c r="HV16" s="11"/>
-      <c r="HW16" s="11"/>
-      <c r="HX16" s="11"/>
-      <c r="HY16" s="11"/>
-      <c r="HZ16" s="11"/>
-      <c r="IA16" s="11"/>
-      <c r="IB16" s="11"/>
-      <c r="IC16" s="11"/>
-      <c r="ID16" s="11"/>
-      <c r="IE16" s="11"/>
-      <c r="IF16" s="11"/>
-      <c r="IG16" s="11"/>
-      <c r="IH16" s="11"/>
-      <c r="II16" s="11"/>
-      <c r="IJ16" s="11"/>
-      <c r="IK16" s="11"/>
-      <c r="IL16" s="11"/>
-      <c r="IM16" s="11"/>
-      <c r="IN16" s="11"/>
-      <c r="IO16" s="11"/>
-      <c r="IP16" s="11"/>
-      <c r="IQ16" s="11"/>
-      <c r="IR16" s="11"/>
-      <c r="IS16" s="11"/>
-      <c r="IT16" s="11"/>
-      <c r="IU16" s="11"/>
-      <c r="IV16" s="11"/>
-      <c r="IW16" s="11"/>
-      <c r="IX16" s="11"/>
-      <c r="IY16" s="11"/>
-      <c r="IZ16" s="11"/>
-      <c r="JA16" s="11"/>
-      <c r="JB16" s="11"/>
-      <c r="JC16" s="11"/>
-      <c r="JD16" s="11"/>
-      <c r="JE16" s="11"/>
-      <c r="JF16" s="11"/>
-      <c r="JG16" s="11"/>
-      <c r="JH16" s="11"/>
-      <c r="JI16" s="11"/>
-      <c r="JJ16" s="11"/>
-      <c r="JK16" s="11"/>
-      <c r="JL16" s="11"/>
-      <c r="JM16" s="11"/>
-      <c r="JN16" s="11"/>
-      <c r="JO16" s="11"/>
-      <c r="JP16" s="11"/>
-      <c r="JQ16" s="11"/>
-      <c r="JR16" s="11"/>
-      <c r="JS16" s="11"/>
-      <c r="JT16" s="11"/>
-      <c r="JU16" s="11"/>
-      <c r="JV16" s="11"/>
-      <c r="JW16" s="11"/>
-      <c r="JX16" s="11"/>
-      <c r="JY16" s="11"/>
-      <c r="JZ16" s="11"/>
-      <c r="KA16" s="11"/>
-      <c r="KB16" s="11"/>
-      <c r="KC16" s="11"/>
-      <c r="KD16" s="11"/>
-      <c r="KE16" s="11"/>
-      <c r="KF16" s="11"/>
-      <c r="KG16" s="11"/>
-      <c r="KH16" s="11"/>
-      <c r="KI16" s="11"/>
-      <c r="KJ16" s="11"/>
-      <c r="KK16" s="11"/>
-      <c r="KL16" s="11"/>
-      <c r="KM16" s="11"/>
-      <c r="KN16" s="11"/>
-      <c r="KO16" s="11"/>
-      <c r="KP16" s="11"/>
-      <c r="KQ16" s="11"/>
-      <c r="KR16" s="11"/>
-      <c r="KS16" s="11"/>
-      <c r="KT16" s="11"/>
-      <c r="KU16" s="11"/>
-      <c r="KV16" s="11"/>
-      <c r="KW16" s="11"/>
-      <c r="KX16" s="11"/>
-      <c r="KY16" s="11"/>
-      <c r="KZ16" s="11"/>
-      <c r="LA16" s="11"/>
-      <c r="LB16" s="11"/>
-      <c r="LC16" s="11"/>
-      <c r="LD16" s="11"/>
-      <c r="LE16" s="11"/>
-      <c r="LF16" s="11"/>
-      <c r="LG16" s="11"/>
-      <c r="LH16" s="11"/>
-      <c r="LI16" s="11"/>
-      <c r="LJ16" s="11"/>
-      <c r="LK16" s="11"/>
-      <c r="LL16" s="11"/>
-      <c r="LM16" s="11"/>
-      <c r="LN16" s="11"/>
-      <c r="LO16" s="11"/>
-      <c r="LP16" s="11"/>
-      <c r="LQ16" s="11"/>
-      <c r="LR16" s="11"/>
-      <c r="LS16" s="11"/>
-      <c r="LT16" s="11"/>
-      <c r="LU16" s="11"/>
-      <c r="LV16" s="11"/>
-      <c r="LW16" s="11"/>
-      <c r="LX16" s="11"/>
-      <c r="LY16" s="11"/>
-      <c r="LZ16" s="11"/>
-      <c r="MA16" s="11"/>
-      <c r="MB16" s="11"/>
-      <c r="MC16" s="11"/>
-      <c r="MD16" s="11"/>
-      <c r="ME16" s="11"/>
-      <c r="MF16" s="11"/>
-      <c r="MG16" s="11"/>
-      <c r="MH16" s="11"/>
-      <c r="MI16" s="11"/>
-      <c r="MJ16" s="11"/>
-      <c r="MK16" s="11"/>
-      <c r="ML16" s="11"/>
-      <c r="MM16" s="11"/>
-      <c r="MN16" s="11"/>
-      <c r="MO16" s="11"/>
-      <c r="MP16" s="11"/>
-      <c r="MQ16" s="11"/>
-      <c r="MR16" s="11"/>
-      <c r="MS16" s="11"/>
-      <c r="MT16" s="11"/>
-      <c r="MU16" s="11"/>
-      <c r="MV16" s="11"/>
-      <c r="MW16" s="11"/>
-      <c r="MX16" s="11"/>
-      <c r="MY16" s="11"/>
-      <c r="MZ16" s="11"/>
-      <c r="NA16" s="11"/>
-      <c r="NB16" s="11"/>
-      <c r="NC16" s="11"/>
-      <c r="ND16" s="11"/>
-      <c r="NE16" s="11"/>
-      <c r="NF16" s="11"/>
-      <c r="NG16" s="11"/>
-      <c r="NH16" s="11"/>
-      <c r="NI16" s="11"/>
-      <c r="NJ16" s="11"/>
-      <c r="NK16" s="11"/>
-      <c r="NL16" s="11"/>
-      <c r="NM16" s="11"/>
-      <c r="NN16" s="11"/>
-      <c r="NO16" s="11"/>
-      <c r="NP16" s="11"/>
-      <c r="NQ16" s="11"/>
-      <c r="NR16" s="11"/>
-      <c r="NS16" s="11"/>
-      <c r="NT16" s="11"/>
-      <c r="NU16" s="11"/>
-      <c r="NV16" s="11"/>
-      <c r="NW16" s="11"/>
-      <c r="NX16" s="11"/>
-      <c r="NY16" s="11"/>
-      <c r="NZ16" s="11"/>
-      <c r="OA16" s="11"/>
-      <c r="OB16" s="11"/>
-      <c r="OC16" s="11"/>
-      <c r="OD16" s="11"/>
-      <c r="OE16" s="11"/>
-      <c r="OF16" s="11"/>
-      <c r="OG16" s="11"/>
-      <c r="OH16" s="11"/>
-      <c r="OI16" s="11"/>
-      <c r="OJ16" s="11"/>
-      <c r="OK16" s="11"/>
-      <c r="OL16" s="11"/>
-      <c r="OM16" s="11"/>
-      <c r="ON16" s="11"/>
-      <c r="OO16" s="11"/>
-      <c r="OP16" s="11"/>
-      <c r="OQ16" s="11"/>
-      <c r="OR16" s="11"/>
-      <c r="OS16" s="11"/>
-      <c r="OT16" s="11"/>
-      <c r="OU16" s="11"/>
-      <c r="OV16" s="11"/>
-      <c r="OW16" s="11"/>
-      <c r="OX16" s="11"/>
-      <c r="OY16" s="11"/>
-      <c r="OZ16" s="11"/>
-      <c r="PA16" s="11"/>
-      <c r="PB16" s="11"/>
-      <c r="PC16" s="11"/>
-      <c r="PD16" s="11"/>
-      <c r="PE16" s="11"/>
-      <c r="PF16" s="11"/>
-      <c r="PG16" s="11"/>
-      <c r="PH16" s="11"/>
-      <c r="PI16" s="11"/>
-      <c r="PJ16" s="11"/>
-      <c r="PK16" s="11"/>
-      <c r="PL16" s="11"/>
-      <c r="PM16" s="11"/>
-      <c r="PN16" s="11"/>
-      <c r="PO16" s="11"/>
-      <c r="PP16" s="11"/>
-      <c r="PQ16" s="11"/>
-      <c r="PR16" s="11"/>
-      <c r="PS16" s="11"/>
-      <c r="PT16" s="11"/>
-      <c r="PU16" s="11"/>
-      <c r="PV16" s="11"/>
-      <c r="PW16" s="11"/>
-      <c r="PX16" s="11"/>
-      <c r="PY16" s="11"/>
-      <c r="PZ16" s="11"/>
-      <c r="QA16" s="11"/>
-      <c r="QB16" s="11"/>
-      <c r="QC16" s="11"/>
-      <c r="QD16" s="11"/>
-      <c r="QE16" s="11"/>
-      <c r="QF16" s="11"/>
-      <c r="QG16" s="11"/>
-      <c r="QH16" s="11"/>
-      <c r="QI16" s="11"/>
-      <c r="QJ16" s="11"/>
-      <c r="QK16" s="11"/>
-      <c r="QL16" s="11"/>
-      <c r="QM16" s="11"/>
-      <c r="QN16" s="11"/>
-      <c r="QO16" s="11"/>
-      <c r="QP16" s="11"/>
-      <c r="QQ16" s="11"/>
-      <c r="QR16" s="11"/>
-      <c r="QS16" s="11"/>
-      <c r="QT16" s="11"/>
-      <c r="QU16" s="11"/>
-      <c r="QV16" s="11"/>
-      <c r="QW16" s="11"/>
-      <c r="QX16" s="11"/>
-      <c r="QY16" s="11"/>
-      <c r="QZ16" s="11"/>
-      <c r="RA16" s="11"/>
-      <c r="RB16" s="11"/>
-      <c r="RC16" s="11"/>
-      <c r="RD16" s="11"/>
-      <c r="RE16" s="11"/>
-      <c r="RF16" s="11"/>
-      <c r="RG16" s="11"/>
-      <c r="RH16" s="11"/>
-      <c r="RI16" s="11"/>
-      <c r="RJ16" s="11"/>
-      <c r="RK16" s="11"/>
-      <c r="RL16" s="11"/>
-      <c r="RM16" s="11"/>
-      <c r="RN16" s="11"/>
-      <c r="RO16" s="11"/>
-      <c r="RP16" s="11"/>
-      <c r="RQ16" s="11"/>
-      <c r="RR16" s="11"/>
-      <c r="RS16" s="11"/>
-      <c r="RT16" s="11"/>
-      <c r="RU16" s="11"/>
-      <c r="RV16" s="11"/>
-      <c r="RW16" s="11"/>
-      <c r="RX16" s="11"/>
-      <c r="RY16" s="11"/>
-      <c r="RZ16" s="11"/>
-      <c r="SA16" s="11"/>
-      <c r="SB16" s="11"/>
-      <c r="SC16" s="11"/>
-      <c r="SD16" s="11"/>
-      <c r="SE16" s="11"/>
-      <c r="SF16" s="11"/>
-      <c r="SG16" s="11"/>
-      <c r="SH16" s="11"/>
-      <c r="SI16" s="11"/>
-      <c r="SJ16" s="11"/>
-      <c r="SK16" s="11"/>
-      <c r="SL16" s="11"/>
-      <c r="SM16" s="11"/>
-      <c r="SN16" s="11"/>
-      <c r="SO16" s="11"/>
-      <c r="SP16" s="11"/>
-      <c r="SQ16" s="11"/>
-      <c r="SR16" s="11"/>
-      <c r="SS16" s="11"/>
-      <c r="ST16" s="11"/>
-      <c r="SU16" s="11"/>
-      <c r="SV16" s="11"/>
-      <c r="SW16" s="11"/>
-      <c r="SX16" s="11"/>
-      <c r="SY16" s="11"/>
-      <c r="SZ16" s="11"/>
-      <c r="TA16" s="11"/>
-      <c r="TB16" s="11"/>
-      <c r="TC16" s="11"/>
-      <c r="TD16" s="11"/>
-      <c r="TE16" s="11"/>
-      <c r="TF16" s="11"/>
-      <c r="TG16" s="11"/>
-      <c r="TH16" s="11"/>
-      <c r="TI16" s="11"/>
-      <c r="TJ16" s="11"/>
-      <c r="TK16" s="11"/>
-      <c r="TL16" s="11"/>
-      <c r="TM16" s="11"/>
-      <c r="TN16" s="11"/>
-      <c r="TO16" s="11"/>
-      <c r="TP16" s="11"/>
-      <c r="TQ16" s="11"/>
-      <c r="TR16" s="11"/>
-      <c r="TS16" s="11"/>
-      <c r="TT16" s="11"/>
-      <c r="TU16" s="11"/>
-      <c r="TV16" s="11"/>
-      <c r="TW16" s="11"/>
-      <c r="TX16" s="11"/>
-      <c r="TY16" s="11"/>
-      <c r="TZ16" s="11"/>
-      <c r="UA16" s="11"/>
-      <c r="UB16" s="11"/>
-      <c r="UC16" s="11"/>
-      <c r="UD16" s="11"/>
-      <c r="UE16" s="11"/>
-      <c r="UF16" s="11"/>
-      <c r="UG16" s="11"/>
-      <c r="UH16" s="11"/>
-      <c r="UI16" s="11"/>
-      <c r="UJ16" s="11"/>
-      <c r="UK16" s="11"/>
-      <c r="UL16" s="11"/>
-      <c r="UM16" s="11"/>
-      <c r="UN16" s="11"/>
-      <c r="UO16" s="11"/>
-      <c r="UP16" s="11"/>
-      <c r="UQ16" s="11"/>
-      <c r="UR16" s="11"/>
-      <c r="US16" s="11"/>
-      <c r="UT16" s="11"/>
-      <c r="UU16" s="11"/>
-      <c r="UV16" s="11"/>
-      <c r="UW16" s="11"/>
-      <c r="UX16" s="11"/>
-      <c r="UY16" s="11"/>
-      <c r="UZ16" s="11"/>
-      <c r="VA16" s="11"/>
-      <c r="VB16" s="11"/>
-      <c r="VC16" s="11"/>
-      <c r="VD16" s="11"/>
-      <c r="VE16" s="11"/>
-      <c r="VF16" s="11"/>
-      <c r="VG16" s="11"/>
-      <c r="VH16" s="11"/>
-      <c r="VI16" s="11"/>
-      <c r="VJ16" s="11"/>
-      <c r="VK16" s="11"/>
-      <c r="VL16" s="11"/>
-      <c r="VM16" s="11"/>
-      <c r="VN16" s="11"/>
-      <c r="VO16" s="11"/>
-      <c r="VP16" s="11"/>
-      <c r="VQ16" s="11"/>
-      <c r="VR16" s="11"/>
-      <c r="VS16" s="11"/>
-      <c r="VT16" s="11"/>
-      <c r="VU16" s="11"/>
-      <c r="VV16" s="11"/>
-      <c r="VW16" s="11"/>
-      <c r="VX16" s="11"/>
-      <c r="VY16" s="11"/>
-      <c r="VZ16" s="11"/>
-      <c r="WA16" s="11"/>
-      <c r="WB16" s="11"/>
-      <c r="WC16" s="11"/>
-      <c r="WD16" s="11"/>
-      <c r="WE16" s="11"/>
-      <c r="WF16" s="11"/>
-      <c r="WG16" s="11"/>
-      <c r="WH16" s="11"/>
-      <c r="WI16" s="11"/>
-      <c r="WJ16" s="11"/>
-      <c r="WK16" s="11"/>
-      <c r="WL16" s="11"/>
-      <c r="WM16" s="11"/>
-      <c r="WN16" s="11"/>
-      <c r="WO16" s="11"/>
-      <c r="WP16" s="11"/>
-      <c r="WQ16" s="11"/>
-      <c r="WR16" s="11"/>
-      <c r="WS16" s="11"/>
-      <c r="WT16" s="11"/>
-      <c r="WU16" s="11"/>
-      <c r="WV16" s="11"/>
-      <c r="WW16" s="11"/>
-      <c r="WX16" s="11"/>
-      <c r="WY16" s="11"/>
-      <c r="WZ16" s="11"/>
-      <c r="XA16" s="11"/>
-      <c r="XB16" s="11"/>
-      <c r="XC16" s="11"/>
-      <c r="XD16" s="11"/>
-      <c r="XE16" s="11"/>
-      <c r="XF16" s="11"/>
-      <c r="XG16" s="11"/>
-      <c r="XH16" s="11"/>
-      <c r="XI16" s="11"/>
-      <c r="XJ16" s="11"/>
-      <c r="XK16" s="11"/>
-      <c r="XL16" s="11"/>
-      <c r="XM16" s="11"/>
-      <c r="XN16" s="11"/>
-      <c r="XO16" s="11"/>
-      <c r="XP16" s="11"/>
-      <c r="XQ16" s="11"/>
-      <c r="XR16" s="11"/>
-      <c r="XS16" s="11"/>
-      <c r="XT16" s="11"/>
-      <c r="XU16" s="11"/>
-      <c r="XV16" s="11"/>
-      <c r="XW16" s="11"/>
-      <c r="XX16" s="11"/>
-      <c r="XY16" s="11"/>
-      <c r="XZ16" s="11"/>
-      <c r="YA16" s="11"/>
-      <c r="YB16" s="11"/>
-      <c r="YC16" s="11"/>
-      <c r="YD16" s="11"/>
-      <c r="YE16" s="11"/>
-      <c r="YF16" s="11"/>
-      <c r="YG16" s="11"/>
-      <c r="YH16" s="11"/>
-      <c r="YI16" s="11"/>
-      <c r="YJ16" s="11"/>
-      <c r="YK16" s="11"/>
-      <c r="YL16" s="11"/>
-      <c r="YM16" s="11"/>
-      <c r="YN16" s="11"/>
-      <c r="YO16" s="11"/>
-      <c r="YP16" s="11"/>
-      <c r="YQ16" s="11"/>
-      <c r="YR16" s="11"/>
-      <c r="YS16" s="11"/>
-      <c r="YT16" s="11"/>
-      <c r="YU16" s="11"/>
-      <c r="YV16" s="11"/>
-      <c r="YW16" s="11"/>
-      <c r="YX16" s="11"/>
-      <c r="YY16" s="11"/>
-      <c r="YZ16" s="11"/>
-      <c r="ZA16" s="11"/>
-      <c r="ZB16" s="11"/>
-      <c r="ZC16" s="11"/>
-      <c r="ZD16" s="11"/>
-      <c r="ZE16" s="11"/>
-      <c r="ZF16" s="11"/>
-      <c r="ZG16" s="11"/>
-      <c r="ZH16" s="11"/>
-      <c r="ZI16" s="11"/>
-      <c r="ZJ16" s="11"/>
-      <c r="ZK16" s="11"/>
-      <c r="ZL16" s="11"/>
-      <c r="ZM16" s="11"/>
-      <c r="ZN16" s="11"/>
-      <c r="ZO16" s="11"/>
-      <c r="ZP16" s="11"/>
-      <c r="ZQ16" s="11"/>
-      <c r="ZR16" s="11"/>
-      <c r="ZS16" s="11"/>
-      <c r="ZT16" s="11"/>
-      <c r="ZU16" s="11"/>
-      <c r="ZV16" s="11"/>
-      <c r="ZW16" s="11"/>
-      <c r="ZX16" s="11"/>
-      <c r="ZY16" s="11"/>
-      <c r="ZZ16" s="11"/>
-      <c r="AAA16" s="11"/>
-      <c r="AAB16" s="11"/>
-      <c r="AAC16" s="11"/>
-      <c r="AAD16" s="11"/>
-      <c r="AAE16" s="11"/>
-      <c r="AAF16" s="11"/>
-      <c r="AAG16" s="11"/>
-      <c r="AAH16" s="11"/>
-      <c r="AAI16" s="11"/>
-      <c r="AAJ16" s="11"/>
-      <c r="AAK16" s="11"/>
-      <c r="AAL16" s="11"/>
-      <c r="AAM16" s="11"/>
-      <c r="AAN16" s="11"/>
-      <c r="AAO16" s="11"/>
-      <c r="AAP16" s="11"/>
-      <c r="AAQ16" s="11"/>
-      <c r="AAR16" s="11"/>
-      <c r="AAS16" s="11"/>
-      <c r="AAT16" s="11"/>
-      <c r="AAU16" s="11"/>
-      <c r="AAV16" s="11"/>
-      <c r="AAW16" s="11"/>
-      <c r="AAX16" s="11"/>
-      <c r="AAY16" s="11"/>
-      <c r="AAZ16" s="11"/>
-      <c r="ABA16" s="11"/>
-      <c r="ABB16" s="11"/>
-      <c r="ABC16" s="11"/>
-      <c r="ABD16" s="11"/>
-      <c r="ABE16" s="11"/>
-      <c r="ABF16" s="11"/>
-      <c r="ABG16" s="11"/>
-      <c r="ABH16" s="11"/>
-      <c r="ABI16" s="11"/>
-      <c r="ABJ16" s="11"/>
-      <c r="ABK16" s="11"/>
-      <c r="ABL16" s="11"/>
-      <c r="ABM16" s="11"/>
-      <c r="ABN16" s="11"/>
-      <c r="ABO16" s="11"/>
-      <c r="ABP16" s="11"/>
-      <c r="ABQ16" s="11"/>
-      <c r="ABR16" s="11"/>
-      <c r="ABS16" s="11"/>
-      <c r="ABT16" s="11"/>
-      <c r="ABU16" s="11"/>
-      <c r="ABV16" s="11"/>
-      <c r="ABW16" s="11"/>
-      <c r="ABX16" s="11"/>
-      <c r="ABY16" s="11"/>
-      <c r="ABZ16" s="11"/>
-      <c r="ACA16" s="11"/>
-      <c r="ACB16" s="11"/>
-      <c r="ACC16" s="11"/>
-      <c r="ACD16" s="11"/>
-      <c r="ACE16" s="11"/>
-      <c r="ACF16" s="11"/>
-      <c r="ACG16" s="11"/>
-      <c r="ACH16" s="11"/>
-      <c r="ACI16" s="11"/>
-      <c r="ACJ16" s="11"/>
-      <c r="ACK16" s="11"/>
-      <c r="ACL16" s="11"/>
-      <c r="ACM16" s="11"/>
-      <c r="ACN16" s="11"/>
-      <c r="ACO16" s="11"/>
-      <c r="ACP16" s="11"/>
-      <c r="ACQ16" s="11"/>
-      <c r="ACR16" s="11"/>
-      <c r="ACS16" s="11"/>
-      <c r="ACT16" s="11"/>
-      <c r="ACU16" s="11"/>
-      <c r="ACV16" s="11"/>
-      <c r="ACW16" s="11"/>
-      <c r="ACX16" s="11"/>
-      <c r="ACY16" s="11"/>
-      <c r="ACZ16" s="11"/>
-      <c r="ADA16" s="11"/>
-      <c r="ADB16" s="11"/>
-      <c r="ADC16" s="11"/>
-      <c r="ADD16" s="11"/>
-      <c r="ADE16" s="11"/>
-      <c r="ADF16" s="11"/>
-      <c r="ADG16" s="11"/>
-      <c r="ADH16" s="11"/>
-      <c r="ADI16" s="11"/>
-      <c r="ADJ16" s="11"/>
-      <c r="ADK16" s="11"/>
-      <c r="ADL16" s="11"/>
-      <c r="ADM16" s="11"/>
-      <c r="ADN16" s="11"/>
-      <c r="ADO16" s="11"/>
-      <c r="ADP16" s="11"/>
-      <c r="ADQ16" s="11"/>
-      <c r="ADR16" s="11"/>
-      <c r="ADS16" s="11"/>
-      <c r="ADT16" s="11"/>
-      <c r="ADU16" s="11"/>
-      <c r="ADV16" s="11"/>
-      <c r="ADW16" s="11"/>
-      <c r="ADX16" s="11"/>
-      <c r="ADY16" s="11"/>
-      <c r="ADZ16" s="11"/>
-      <c r="AEA16" s="11"/>
-      <c r="AEB16" s="11"/>
-      <c r="AEC16" s="11"/>
-      <c r="AED16" s="11"/>
-      <c r="AEE16" s="11"/>
-      <c r="AEF16" s="11"/>
-      <c r="AEG16" s="11"/>
-      <c r="AEH16" s="11"/>
-      <c r="AEI16" s="11"/>
-      <c r="AEJ16" s="11"/>
-      <c r="AEK16" s="11"/>
-      <c r="AEL16" s="11"/>
-      <c r="AEM16" s="11"/>
-      <c r="AEN16" s="11"/>
-      <c r="AEO16" s="11"/>
-      <c r="AEP16" s="11"/>
-      <c r="AEQ16" s="11"/>
-      <c r="AER16" s="11"/>
-      <c r="AES16" s="11"/>
-      <c r="AET16" s="11"/>
-      <c r="AEU16" s="11"/>
-      <c r="AEV16" s="11"/>
-      <c r="AEW16" s="11"/>
-      <c r="AEX16" s="11"/>
-      <c r="AEY16" s="11"/>
-      <c r="AEZ16" s="11"/>
-      <c r="AFA16" s="11"/>
-      <c r="AFB16" s="11"/>
-      <c r="AFC16" s="11"/>
-      <c r="AFD16" s="11"/>
-      <c r="AFE16" s="11"/>
-      <c r="AFF16" s="11"/>
-      <c r="AFG16" s="11"/>
-      <c r="AFH16" s="11"/>
-      <c r="AFI16" s="11"/>
-      <c r="AFJ16" s="11"/>
-      <c r="AFK16" s="11"/>
-      <c r="AFL16" s="11"/>
-      <c r="AFM16" s="11"/>
-      <c r="AFN16" s="11"/>
-      <c r="AFO16" s="11"/>
-      <c r="AFP16" s="11"/>
-      <c r="AFQ16" s="11"/>
-      <c r="AFR16" s="11"/>
-      <c r="AFS16" s="11"/>
-      <c r="AFT16" s="11"/>
-      <c r="AFU16" s="11"/>
-      <c r="AFV16" s="11"/>
-      <c r="AFW16" s="11"/>
-      <c r="AFX16" s="11"/>
-      <c r="AFY16" s="11"/>
-      <c r="AFZ16" s="11"/>
-      <c r="AGA16" s="11"/>
-      <c r="AGB16" s="11"/>
-      <c r="AGC16" s="11"/>
-      <c r="AGD16" s="11"/>
-      <c r="AGE16" s="11"/>
-      <c r="AGF16" s="11"/>
-      <c r="AGG16" s="11"/>
-      <c r="AGH16" s="11"/>
-      <c r="AGI16" s="11"/>
-      <c r="AGJ16" s="11"/>
-      <c r="AGK16" s="11"/>
-      <c r="AGL16" s="11"/>
-      <c r="AGM16" s="11"/>
-      <c r="AGN16" s="11"/>
-      <c r="AGO16" s="11"/>
-      <c r="AGP16" s="11"/>
-      <c r="AGQ16" s="11"/>
-      <c r="AGR16" s="11"/>
-      <c r="AGS16" s="11"/>
-      <c r="AGT16" s="11"/>
-      <c r="AGU16" s="11"/>
-      <c r="AGV16" s="11"/>
-      <c r="AGW16" s="11"/>
-      <c r="AGX16" s="11"/>
-      <c r="AGY16" s="11"/>
-      <c r="AGZ16" s="11"/>
-      <c r="AHA16" s="11"/>
-      <c r="AHB16" s="11"/>
-      <c r="AHC16" s="11"/>
-      <c r="AHD16" s="11"/>
-      <c r="AHE16" s="11"/>
-      <c r="AHF16" s="11"/>
-      <c r="AHG16" s="11"/>
-      <c r="AHH16" s="11"/>
-      <c r="AHI16" s="11"/>
-      <c r="AHJ16" s="11"/>
-      <c r="AHK16" s="11"/>
-      <c r="AHL16" s="11"/>
-      <c r="AHM16" s="11"/>
-      <c r="AHN16" s="11"/>
-      <c r="AHO16" s="11"/>
-      <c r="AHP16" s="11"/>
-      <c r="AHQ16" s="11"/>
-      <c r="AHR16" s="11"/>
-      <c r="AHS16" s="11"/>
-      <c r="AHT16" s="11"/>
-      <c r="AHU16" s="11"/>
-      <c r="AHV16" s="11"/>
-      <c r="AHW16" s="11"/>
-      <c r="AHX16" s="11"/>
-      <c r="AHY16" s="11"/>
-      <c r="AHZ16" s="11"/>
-      <c r="AIA16" s="11"/>
-      <c r="AIB16" s="11"/>
-      <c r="AIC16" s="11"/>
-      <c r="AID16" s="11"/>
-      <c r="AIE16" s="11"/>
-      <c r="AIF16" s="11"/>
-      <c r="AIG16" s="11"/>
-      <c r="AIH16" s="11"/>
-      <c r="AII16" s="11"/>
-      <c r="AIJ16" s="11"/>
-      <c r="AIK16" s="11"/>
-      <c r="AIL16" s="11"/>
-      <c r="AIM16" s="11"/>
-      <c r="AIN16" s="11"/>
-      <c r="AIO16" s="11"/>
-      <c r="AIP16" s="11"/>
-      <c r="AIQ16" s="11"/>
-      <c r="AIR16" s="11"/>
-      <c r="AIS16" s="11"/>
-      <c r="AIT16" s="11"/>
-      <c r="AIU16" s="11"/>
-      <c r="AIV16" s="11"/>
-      <c r="AIW16" s="11"/>
-      <c r="AIX16" s="11"/>
-      <c r="AIY16" s="11"/>
-      <c r="AIZ16" s="11"/>
-      <c r="AJA16" s="11"/>
-      <c r="AJB16" s="11"/>
-      <c r="AJC16" s="11"/>
-      <c r="AJD16" s="11"/>
-      <c r="AJE16" s="11"/>
-      <c r="AJF16" s="11"/>
-      <c r="AJG16" s="11"/>
-      <c r="AJH16" s="11"/>
-      <c r="AJI16" s="11"/>
-      <c r="AJJ16" s="11"/>
-      <c r="AJK16" s="11"/>
-      <c r="AJL16" s="11"/>
-      <c r="AJM16" s="11"/>
-      <c r="AJN16" s="11"/>
-      <c r="AJO16" s="11"/>
-      <c r="AJP16" s="11"/>
-      <c r="AJQ16" s="11"/>
-      <c r="AJR16" s="11"/>
-      <c r="AJS16" s="11"/>
-      <c r="AJT16" s="11"/>
-      <c r="AJU16" s="11"/>
-      <c r="AJV16" s="11"/>
-      <c r="AJW16" s="11"/>
-      <c r="AJX16" s="11"/>
-      <c r="AJY16" s="11"/>
-      <c r="AJZ16" s="11"/>
-      <c r="AKA16" s="11"/>
-      <c r="AKB16" s="11"/>
-      <c r="AKC16" s="11"/>
-      <c r="AKD16" s="11"/>
-      <c r="AKE16" s="11"/>
-      <c r="AKF16" s="11"/>
-      <c r="AKG16" s="11"/>
-      <c r="AKH16" s="11"/>
-      <c r="AKI16" s="11"/>
-      <c r="AKJ16" s="11"/>
-      <c r="AKK16" s="11"/>
-      <c r="AKL16" s="11"/>
-      <c r="AKM16" s="11"/>
-      <c r="AKN16" s="11"/>
-      <c r="AKO16" s="11"/>
-      <c r="AKP16" s="11"/>
-      <c r="AKQ16" s="11"/>
-      <c r="AKR16" s="11"/>
-      <c r="AKS16" s="11"/>
-      <c r="AKT16" s="11"/>
-      <c r="AKU16" s="11"/>
-      <c r="AKV16" s="11"/>
-      <c r="AKW16" s="11"/>
-      <c r="AKX16" s="11"/>
-      <c r="AKY16" s="11"/>
-      <c r="AKZ16" s="11"/>
-      <c r="ALA16" s="11"/>
-      <c r="ALB16" s="11"/>
-      <c r="ALC16" s="11"/>
-      <c r="ALD16" s="11"/>
-      <c r="ALE16" s="11"/>
-      <c r="ALF16" s="11"/>
-      <c r="ALG16" s="11"/>
-      <c r="ALH16" s="11"/>
-      <c r="ALI16" s="11"/>
-      <c r="ALJ16" s="11"/>
-      <c r="ALK16" s="11"/>
-      <c r="ALL16" s="11"/>
-      <c r="ALM16" s="11"/>
-      <c r="ALN16" s="11"/>
-      <c r="ALO16" s="11"/>
-      <c r="ALP16" s="11"/>
-      <c r="ALQ16" s="11"/>
-      <c r="ALR16" s="11"/>
-      <c r="ALS16" s="11"/>
-      <c r="ALT16" s="11"/>
-      <c r="ALU16" s="11"/>
-      <c r="ALV16" s="11"/>
-      <c r="ALW16" s="11"/>
-      <c r="ALX16" s="11"/>
-      <c r="ALY16" s="11"/>
-      <c r="ALZ16" s="11"/>
-      <c r="AMA16" s="11"/>
-      <c r="AMB16" s="11"/>
-      <c r="AMC16" s="11"/>
-      <c r="AMD16" s="11"/>
-      <c r="AME16" s="11"/>
-      <c r="AMF16" s="11"/>
-      <c r="AMG16" s="11"/>
-      <c r="AMH16" s="11"/>
-      <c r="AMI16" s="11"/>
-      <c r="AMJ16" s="11"/>
-      <c r="AMK16" s="11"/>
+      <c r="J16" s="15">
+        <v>2</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="17" spans="1:1025" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1025" s="13" customFormat="1">
       <c r="A17" s="10">
         <v>3.17</v>
       </c>
@@ -14569,7 +12560,9 @@
       <c r="J17" s="11">
         <v>6</v>
       </c>
-      <c r="K17" s="11"/>
+      <c r="K17" s="11" t="s">
+        <v>12</v>
+      </c>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
@@ -15585,1057 +13578,44 @@
       <c r="AMJ17" s="11"/>
       <c r="AMK17" s="11"/>
     </row>
-    <row r="18" spans="1:1025" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+    <row r="18" spans="1:1025" s="15" customFormat="1">
+      <c r="A18" s="14">
         <v>3.12</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="15">
         <v>2</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="15">
         <v>4</v>
       </c>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11">
+      <c r="J18" s="15">
         <v>4.5</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="11"/>
-      <c r="AD18" s="11"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="11"/>
-      <c r="AH18" s="11"/>
-      <c r="AI18" s="11"/>
-      <c r="AJ18" s="11"/>
-      <c r="AK18" s="11"/>
-      <c r="AL18" s="11"/>
-      <c r="AM18" s="11"/>
-      <c r="AN18" s="11"/>
-      <c r="AO18" s="11"/>
-      <c r="AP18" s="11"/>
-      <c r="AQ18" s="11"/>
-      <c r="AR18" s="11"/>
-      <c r="AS18" s="11"/>
-      <c r="AT18" s="11"/>
-      <c r="AU18" s="11"/>
-      <c r="AV18" s="11"/>
-      <c r="AW18" s="11"/>
-      <c r="AX18" s="11"/>
-      <c r="AY18" s="11"/>
-      <c r="AZ18" s="11"/>
-      <c r="BA18" s="11"/>
-      <c r="BB18" s="11"/>
-      <c r="BC18" s="11"/>
-      <c r="BD18" s="11"/>
-      <c r="BE18" s="11"/>
-      <c r="BF18" s="11"/>
-      <c r="BG18" s="11"/>
-      <c r="BH18" s="11"/>
-      <c r="BI18" s="11"/>
-      <c r="BJ18" s="11"/>
-      <c r="BK18" s="11"/>
-      <c r="BL18" s="11"/>
-      <c r="BM18" s="11"/>
-      <c r="BN18" s="11"/>
-      <c r="BO18" s="11"/>
-      <c r="BP18" s="11"/>
-      <c r="BQ18" s="11"/>
-      <c r="BR18" s="11"/>
-      <c r="BS18" s="11"/>
-      <c r="BT18" s="11"/>
-      <c r="BU18" s="11"/>
-      <c r="BV18" s="11"/>
-      <c r="BW18" s="11"/>
-      <c r="BX18" s="11"/>
-      <c r="BY18" s="11"/>
-      <c r="BZ18" s="11"/>
-      <c r="CA18" s="11"/>
-      <c r="CB18" s="11"/>
-      <c r="CC18" s="11"/>
-      <c r="CD18" s="11"/>
-      <c r="CE18" s="11"/>
-      <c r="CF18" s="11"/>
-      <c r="CG18" s="11"/>
-      <c r="CH18" s="11"/>
-      <c r="CI18" s="11"/>
-      <c r="CJ18" s="11"/>
-      <c r="CK18" s="11"/>
-      <c r="CL18" s="11"/>
-      <c r="CM18" s="11"/>
-      <c r="CN18" s="11"/>
-      <c r="CO18" s="11"/>
-      <c r="CP18" s="11"/>
-      <c r="CQ18" s="11"/>
-      <c r="CR18" s="11"/>
-      <c r="CS18" s="11"/>
-      <c r="CT18" s="11"/>
-      <c r="CU18" s="11"/>
-      <c r="CV18" s="11"/>
-      <c r="CW18" s="11"/>
-      <c r="CX18" s="11"/>
-      <c r="CY18" s="11"/>
-      <c r="CZ18" s="11"/>
-      <c r="DA18" s="11"/>
-      <c r="DB18" s="11"/>
-      <c r="DC18" s="11"/>
-      <c r="DD18" s="11"/>
-      <c r="DE18" s="11"/>
-      <c r="DF18" s="11"/>
-      <c r="DG18" s="11"/>
-      <c r="DH18" s="11"/>
-      <c r="DI18" s="11"/>
-      <c r="DJ18" s="11"/>
-      <c r="DK18" s="11"/>
-      <c r="DL18" s="11"/>
-      <c r="DM18" s="11"/>
-      <c r="DN18" s="11"/>
-      <c r="DO18" s="11"/>
-      <c r="DP18" s="11"/>
-      <c r="DQ18" s="11"/>
-      <c r="DR18" s="11"/>
-      <c r="DS18" s="11"/>
-      <c r="DT18" s="11"/>
-      <c r="DU18" s="11"/>
-      <c r="DV18" s="11"/>
-      <c r="DW18" s="11"/>
-      <c r="DX18" s="11"/>
-      <c r="DY18" s="11"/>
-      <c r="DZ18" s="11"/>
-      <c r="EA18" s="11"/>
-      <c r="EB18" s="11"/>
-      <c r="EC18" s="11"/>
-      <c r="ED18" s="11"/>
-      <c r="EE18" s="11"/>
-      <c r="EF18" s="11"/>
-      <c r="EG18" s="11"/>
-      <c r="EH18" s="11"/>
-      <c r="EI18" s="11"/>
-      <c r="EJ18" s="11"/>
-      <c r="EK18" s="11"/>
-      <c r="EL18" s="11"/>
-      <c r="EM18" s="11"/>
-      <c r="EN18" s="11"/>
-      <c r="EO18" s="11"/>
-      <c r="EP18" s="11"/>
-      <c r="EQ18" s="11"/>
-      <c r="ER18" s="11"/>
-      <c r="ES18" s="11"/>
-      <c r="ET18" s="11"/>
-      <c r="EU18" s="11"/>
-      <c r="EV18" s="11"/>
-      <c r="EW18" s="11"/>
-      <c r="EX18" s="11"/>
-      <c r="EY18" s="11"/>
-      <c r="EZ18" s="11"/>
-      <c r="FA18" s="11"/>
-      <c r="FB18" s="11"/>
-      <c r="FC18" s="11"/>
-      <c r="FD18" s="11"/>
-      <c r="FE18" s="11"/>
-      <c r="FF18" s="11"/>
-      <c r="FG18" s="11"/>
-      <c r="FH18" s="11"/>
-      <c r="FI18" s="11"/>
-      <c r="FJ18" s="11"/>
-      <c r="FK18" s="11"/>
-      <c r="FL18" s="11"/>
-      <c r="FM18" s="11"/>
-      <c r="FN18" s="11"/>
-      <c r="FO18" s="11"/>
-      <c r="FP18" s="11"/>
-      <c r="FQ18" s="11"/>
-      <c r="FR18" s="11"/>
-      <c r="FS18" s="11"/>
-      <c r="FT18" s="11"/>
-      <c r="FU18" s="11"/>
-      <c r="FV18" s="11"/>
-      <c r="FW18" s="11"/>
-      <c r="FX18" s="11"/>
-      <c r="FY18" s="11"/>
-      <c r="FZ18" s="11"/>
-      <c r="GA18" s="11"/>
-      <c r="GB18" s="11"/>
-      <c r="GC18" s="11"/>
-      <c r="GD18" s="11"/>
-      <c r="GE18" s="11"/>
-      <c r="GF18" s="11"/>
-      <c r="GG18" s="11"/>
-      <c r="GH18" s="11"/>
-      <c r="GI18" s="11"/>
-      <c r="GJ18" s="11"/>
-      <c r="GK18" s="11"/>
-      <c r="GL18" s="11"/>
-      <c r="GM18" s="11"/>
-      <c r="GN18" s="11"/>
-      <c r="GO18" s="11"/>
-      <c r="GP18" s="11"/>
-      <c r="GQ18" s="11"/>
-      <c r="GR18" s="11"/>
-      <c r="GS18" s="11"/>
-      <c r="GT18" s="11"/>
-      <c r="GU18" s="11"/>
-      <c r="GV18" s="11"/>
-      <c r="GW18" s="11"/>
-      <c r="GX18" s="11"/>
-      <c r="GY18" s="11"/>
-      <c r="GZ18" s="11"/>
-      <c r="HA18" s="11"/>
-      <c r="HB18" s="11"/>
-      <c r="HC18" s="11"/>
-      <c r="HD18" s="11"/>
-      <c r="HE18" s="11"/>
-      <c r="HF18" s="11"/>
-      <c r="HG18" s="11"/>
-      <c r="HH18" s="11"/>
-      <c r="HI18" s="11"/>
-      <c r="HJ18" s="11"/>
-      <c r="HK18" s="11"/>
-      <c r="HL18" s="11"/>
-      <c r="HM18" s="11"/>
-      <c r="HN18" s="11"/>
-      <c r="HO18" s="11"/>
-      <c r="HP18" s="11"/>
-      <c r="HQ18" s="11"/>
-      <c r="HR18" s="11"/>
-      <c r="HS18" s="11"/>
-      <c r="HT18" s="11"/>
-      <c r="HU18" s="11"/>
-      <c r="HV18" s="11"/>
-      <c r="HW18" s="11"/>
-      <c r="HX18" s="11"/>
-      <c r="HY18" s="11"/>
-      <c r="HZ18" s="11"/>
-      <c r="IA18" s="11"/>
-      <c r="IB18" s="11"/>
-      <c r="IC18" s="11"/>
-      <c r="ID18" s="11"/>
-      <c r="IE18" s="11"/>
-      <c r="IF18" s="11"/>
-      <c r="IG18" s="11"/>
-      <c r="IH18" s="11"/>
-      <c r="II18" s="11"/>
-      <c r="IJ18" s="11"/>
-      <c r="IK18" s="11"/>
-      <c r="IL18" s="11"/>
-      <c r="IM18" s="11"/>
-      <c r="IN18" s="11"/>
-      <c r="IO18" s="11"/>
-      <c r="IP18" s="11"/>
-      <c r="IQ18" s="11"/>
-      <c r="IR18" s="11"/>
-      <c r="IS18" s="11"/>
-      <c r="IT18" s="11"/>
-      <c r="IU18" s="11"/>
-      <c r="IV18" s="11"/>
-      <c r="IW18" s="11"/>
-      <c r="IX18" s="11"/>
-      <c r="IY18" s="11"/>
-      <c r="IZ18" s="11"/>
-      <c r="JA18" s="11"/>
-      <c r="JB18" s="11"/>
-      <c r="JC18" s="11"/>
-      <c r="JD18" s="11"/>
-      <c r="JE18" s="11"/>
-      <c r="JF18" s="11"/>
-      <c r="JG18" s="11"/>
-      <c r="JH18" s="11"/>
-      <c r="JI18" s="11"/>
-      <c r="JJ18" s="11"/>
-      <c r="JK18" s="11"/>
-      <c r="JL18" s="11"/>
-      <c r="JM18" s="11"/>
-      <c r="JN18" s="11"/>
-      <c r="JO18" s="11"/>
-      <c r="JP18" s="11"/>
-      <c r="JQ18" s="11"/>
-      <c r="JR18" s="11"/>
-      <c r="JS18" s="11"/>
-      <c r="JT18" s="11"/>
-      <c r="JU18" s="11"/>
-      <c r="JV18" s="11"/>
-      <c r="JW18" s="11"/>
-      <c r="JX18" s="11"/>
-      <c r="JY18" s="11"/>
-      <c r="JZ18" s="11"/>
-      <c r="KA18" s="11"/>
-      <c r="KB18" s="11"/>
-      <c r="KC18" s="11"/>
-      <c r="KD18" s="11"/>
-      <c r="KE18" s="11"/>
-      <c r="KF18" s="11"/>
-      <c r="KG18" s="11"/>
-      <c r="KH18" s="11"/>
-      <c r="KI18" s="11"/>
-      <c r="KJ18" s="11"/>
-      <c r="KK18" s="11"/>
-      <c r="KL18" s="11"/>
-      <c r="KM18" s="11"/>
-      <c r="KN18" s="11"/>
-      <c r="KO18" s="11"/>
-      <c r="KP18" s="11"/>
-      <c r="KQ18" s="11"/>
-      <c r="KR18" s="11"/>
-      <c r="KS18" s="11"/>
-      <c r="KT18" s="11"/>
-      <c r="KU18" s="11"/>
-      <c r="KV18" s="11"/>
-      <c r="KW18" s="11"/>
-      <c r="KX18" s="11"/>
-      <c r="KY18" s="11"/>
-      <c r="KZ18" s="11"/>
-      <c r="LA18" s="11"/>
-      <c r="LB18" s="11"/>
-      <c r="LC18" s="11"/>
-      <c r="LD18" s="11"/>
-      <c r="LE18" s="11"/>
-      <c r="LF18" s="11"/>
-      <c r="LG18" s="11"/>
-      <c r="LH18" s="11"/>
-      <c r="LI18" s="11"/>
-      <c r="LJ18" s="11"/>
-      <c r="LK18" s="11"/>
-      <c r="LL18" s="11"/>
-      <c r="LM18" s="11"/>
-      <c r="LN18" s="11"/>
-      <c r="LO18" s="11"/>
-      <c r="LP18" s="11"/>
-      <c r="LQ18" s="11"/>
-      <c r="LR18" s="11"/>
-      <c r="LS18" s="11"/>
-      <c r="LT18" s="11"/>
-      <c r="LU18" s="11"/>
-      <c r="LV18" s="11"/>
-      <c r="LW18" s="11"/>
-      <c r="LX18" s="11"/>
-      <c r="LY18" s="11"/>
-      <c r="LZ18" s="11"/>
-      <c r="MA18" s="11"/>
-      <c r="MB18" s="11"/>
-      <c r="MC18" s="11"/>
-      <c r="MD18" s="11"/>
-      <c r="ME18" s="11"/>
-      <c r="MF18" s="11"/>
-      <c r="MG18" s="11"/>
-      <c r="MH18" s="11"/>
-      <c r="MI18" s="11"/>
-      <c r="MJ18" s="11"/>
-      <c r="MK18" s="11"/>
-      <c r="ML18" s="11"/>
-      <c r="MM18" s="11"/>
-      <c r="MN18" s="11"/>
-      <c r="MO18" s="11"/>
-      <c r="MP18" s="11"/>
-      <c r="MQ18" s="11"/>
-      <c r="MR18" s="11"/>
-      <c r="MS18" s="11"/>
-      <c r="MT18" s="11"/>
-      <c r="MU18" s="11"/>
-      <c r="MV18" s="11"/>
-      <c r="MW18" s="11"/>
-      <c r="MX18" s="11"/>
-      <c r="MY18" s="11"/>
-      <c r="MZ18" s="11"/>
-      <c r="NA18" s="11"/>
-      <c r="NB18" s="11"/>
-      <c r="NC18" s="11"/>
-      <c r="ND18" s="11"/>
-      <c r="NE18" s="11"/>
-      <c r="NF18" s="11"/>
-      <c r="NG18" s="11"/>
-      <c r="NH18" s="11"/>
-      <c r="NI18" s="11"/>
-      <c r="NJ18" s="11"/>
-      <c r="NK18" s="11"/>
-      <c r="NL18" s="11"/>
-      <c r="NM18" s="11"/>
-      <c r="NN18" s="11"/>
-      <c r="NO18" s="11"/>
-      <c r="NP18" s="11"/>
-      <c r="NQ18" s="11"/>
-      <c r="NR18" s="11"/>
-      <c r="NS18" s="11"/>
-      <c r="NT18" s="11"/>
-      <c r="NU18" s="11"/>
-      <c r="NV18" s="11"/>
-      <c r="NW18" s="11"/>
-      <c r="NX18" s="11"/>
-      <c r="NY18" s="11"/>
-      <c r="NZ18" s="11"/>
-      <c r="OA18" s="11"/>
-      <c r="OB18" s="11"/>
-      <c r="OC18" s="11"/>
-      <c r="OD18" s="11"/>
-      <c r="OE18" s="11"/>
-      <c r="OF18" s="11"/>
-      <c r="OG18" s="11"/>
-      <c r="OH18" s="11"/>
-      <c r="OI18" s="11"/>
-      <c r="OJ18" s="11"/>
-      <c r="OK18" s="11"/>
-      <c r="OL18" s="11"/>
-      <c r="OM18" s="11"/>
-      <c r="ON18" s="11"/>
-      <c r="OO18" s="11"/>
-      <c r="OP18" s="11"/>
-      <c r="OQ18" s="11"/>
-      <c r="OR18" s="11"/>
-      <c r="OS18" s="11"/>
-      <c r="OT18" s="11"/>
-      <c r="OU18" s="11"/>
-      <c r="OV18" s="11"/>
-      <c r="OW18" s="11"/>
-      <c r="OX18" s="11"/>
-      <c r="OY18" s="11"/>
-      <c r="OZ18" s="11"/>
-      <c r="PA18" s="11"/>
-      <c r="PB18" s="11"/>
-      <c r="PC18" s="11"/>
-      <c r="PD18" s="11"/>
-      <c r="PE18" s="11"/>
-      <c r="PF18" s="11"/>
-      <c r="PG18" s="11"/>
-      <c r="PH18" s="11"/>
-      <c r="PI18" s="11"/>
-      <c r="PJ18" s="11"/>
-      <c r="PK18" s="11"/>
-      <c r="PL18" s="11"/>
-      <c r="PM18" s="11"/>
-      <c r="PN18" s="11"/>
-      <c r="PO18" s="11"/>
-      <c r="PP18" s="11"/>
-      <c r="PQ18" s="11"/>
-      <c r="PR18" s="11"/>
-      <c r="PS18" s="11"/>
-      <c r="PT18" s="11"/>
-      <c r="PU18" s="11"/>
-      <c r="PV18" s="11"/>
-      <c r="PW18" s="11"/>
-      <c r="PX18" s="11"/>
-      <c r="PY18" s="11"/>
-      <c r="PZ18" s="11"/>
-      <c r="QA18" s="11"/>
-      <c r="QB18" s="11"/>
-      <c r="QC18" s="11"/>
-      <c r="QD18" s="11"/>
-      <c r="QE18" s="11"/>
-      <c r="QF18" s="11"/>
-      <c r="QG18" s="11"/>
-      <c r="QH18" s="11"/>
-      <c r="QI18" s="11"/>
-      <c r="QJ18" s="11"/>
-      <c r="QK18" s="11"/>
-      <c r="QL18" s="11"/>
-      <c r="QM18" s="11"/>
-      <c r="QN18" s="11"/>
-      <c r="QO18" s="11"/>
-      <c r="QP18" s="11"/>
-      <c r="QQ18" s="11"/>
-      <c r="QR18" s="11"/>
-      <c r="QS18" s="11"/>
-      <c r="QT18" s="11"/>
-      <c r="QU18" s="11"/>
-      <c r="QV18" s="11"/>
-      <c r="QW18" s="11"/>
-      <c r="QX18" s="11"/>
-      <c r="QY18" s="11"/>
-      <c r="QZ18" s="11"/>
-      <c r="RA18" s="11"/>
-      <c r="RB18" s="11"/>
-      <c r="RC18" s="11"/>
-      <c r="RD18" s="11"/>
-      <c r="RE18" s="11"/>
-      <c r="RF18" s="11"/>
-      <c r="RG18" s="11"/>
-      <c r="RH18" s="11"/>
-      <c r="RI18" s="11"/>
-      <c r="RJ18" s="11"/>
-      <c r="RK18" s="11"/>
-      <c r="RL18" s="11"/>
-      <c r="RM18" s="11"/>
-      <c r="RN18" s="11"/>
-      <c r="RO18" s="11"/>
-      <c r="RP18" s="11"/>
-      <c r="RQ18" s="11"/>
-      <c r="RR18" s="11"/>
-      <c r="RS18" s="11"/>
-      <c r="RT18" s="11"/>
-      <c r="RU18" s="11"/>
-      <c r="RV18" s="11"/>
-      <c r="RW18" s="11"/>
-      <c r="RX18" s="11"/>
-      <c r="RY18" s="11"/>
-      <c r="RZ18" s="11"/>
-      <c r="SA18" s="11"/>
-      <c r="SB18" s="11"/>
-      <c r="SC18" s="11"/>
-      <c r="SD18" s="11"/>
-      <c r="SE18" s="11"/>
-      <c r="SF18" s="11"/>
-      <c r="SG18" s="11"/>
-      <c r="SH18" s="11"/>
-      <c r="SI18" s="11"/>
-      <c r="SJ18" s="11"/>
-      <c r="SK18" s="11"/>
-      <c r="SL18" s="11"/>
-      <c r="SM18" s="11"/>
-      <c r="SN18" s="11"/>
-      <c r="SO18" s="11"/>
-      <c r="SP18" s="11"/>
-      <c r="SQ18" s="11"/>
-      <c r="SR18" s="11"/>
-      <c r="SS18" s="11"/>
-      <c r="ST18" s="11"/>
-      <c r="SU18" s="11"/>
-      <c r="SV18" s="11"/>
-      <c r="SW18" s="11"/>
-      <c r="SX18" s="11"/>
-      <c r="SY18" s="11"/>
-      <c r="SZ18" s="11"/>
-      <c r="TA18" s="11"/>
-      <c r="TB18" s="11"/>
-      <c r="TC18" s="11"/>
-      <c r="TD18" s="11"/>
-      <c r="TE18" s="11"/>
-      <c r="TF18" s="11"/>
-      <c r="TG18" s="11"/>
-      <c r="TH18" s="11"/>
-      <c r="TI18" s="11"/>
-      <c r="TJ18" s="11"/>
-      <c r="TK18" s="11"/>
-      <c r="TL18" s="11"/>
-      <c r="TM18" s="11"/>
-      <c r="TN18" s="11"/>
-      <c r="TO18" s="11"/>
-      <c r="TP18" s="11"/>
-      <c r="TQ18" s="11"/>
-      <c r="TR18" s="11"/>
-      <c r="TS18" s="11"/>
-      <c r="TT18" s="11"/>
-      <c r="TU18" s="11"/>
-      <c r="TV18" s="11"/>
-      <c r="TW18" s="11"/>
-      <c r="TX18" s="11"/>
-      <c r="TY18" s="11"/>
-      <c r="TZ18" s="11"/>
-      <c r="UA18" s="11"/>
-      <c r="UB18" s="11"/>
-      <c r="UC18" s="11"/>
-      <c r="UD18" s="11"/>
-      <c r="UE18" s="11"/>
-      <c r="UF18" s="11"/>
-      <c r="UG18" s="11"/>
-      <c r="UH18" s="11"/>
-      <c r="UI18" s="11"/>
-      <c r="UJ18" s="11"/>
-      <c r="UK18" s="11"/>
-      <c r="UL18" s="11"/>
-      <c r="UM18" s="11"/>
-      <c r="UN18" s="11"/>
-      <c r="UO18" s="11"/>
-      <c r="UP18" s="11"/>
-      <c r="UQ18" s="11"/>
-      <c r="UR18" s="11"/>
-      <c r="US18" s="11"/>
-      <c r="UT18" s="11"/>
-      <c r="UU18" s="11"/>
-      <c r="UV18" s="11"/>
-      <c r="UW18" s="11"/>
-      <c r="UX18" s="11"/>
-      <c r="UY18" s="11"/>
-      <c r="UZ18" s="11"/>
-      <c r="VA18" s="11"/>
-      <c r="VB18" s="11"/>
-      <c r="VC18" s="11"/>
-      <c r="VD18" s="11"/>
-      <c r="VE18" s="11"/>
-      <c r="VF18" s="11"/>
-      <c r="VG18" s="11"/>
-      <c r="VH18" s="11"/>
-      <c r="VI18" s="11"/>
-      <c r="VJ18" s="11"/>
-      <c r="VK18" s="11"/>
-      <c r="VL18" s="11"/>
-      <c r="VM18" s="11"/>
-      <c r="VN18" s="11"/>
-      <c r="VO18" s="11"/>
-      <c r="VP18" s="11"/>
-      <c r="VQ18" s="11"/>
-      <c r="VR18" s="11"/>
-      <c r="VS18" s="11"/>
-      <c r="VT18" s="11"/>
-      <c r="VU18" s="11"/>
-      <c r="VV18" s="11"/>
-      <c r="VW18" s="11"/>
-      <c r="VX18" s="11"/>
-      <c r="VY18" s="11"/>
-      <c r="VZ18" s="11"/>
-      <c r="WA18" s="11"/>
-      <c r="WB18" s="11"/>
-      <c r="WC18" s="11"/>
-      <c r="WD18" s="11"/>
-      <c r="WE18" s="11"/>
-      <c r="WF18" s="11"/>
-      <c r="WG18" s="11"/>
-      <c r="WH18" s="11"/>
-      <c r="WI18" s="11"/>
-      <c r="WJ18" s="11"/>
-      <c r="WK18" s="11"/>
-      <c r="WL18" s="11"/>
-      <c r="WM18" s="11"/>
-      <c r="WN18" s="11"/>
-      <c r="WO18" s="11"/>
-      <c r="WP18" s="11"/>
-      <c r="WQ18" s="11"/>
-      <c r="WR18" s="11"/>
-      <c r="WS18" s="11"/>
-      <c r="WT18" s="11"/>
-      <c r="WU18" s="11"/>
-      <c r="WV18" s="11"/>
-      <c r="WW18" s="11"/>
-      <c r="WX18" s="11"/>
-      <c r="WY18" s="11"/>
-      <c r="WZ18" s="11"/>
-      <c r="XA18" s="11"/>
-      <c r="XB18" s="11"/>
-      <c r="XC18" s="11"/>
-      <c r="XD18" s="11"/>
-      <c r="XE18" s="11"/>
-      <c r="XF18" s="11"/>
-      <c r="XG18" s="11"/>
-      <c r="XH18" s="11"/>
-      <c r="XI18" s="11"/>
-      <c r="XJ18" s="11"/>
-      <c r="XK18" s="11"/>
-      <c r="XL18" s="11"/>
-      <c r="XM18" s="11"/>
-      <c r="XN18" s="11"/>
-      <c r="XO18" s="11"/>
-      <c r="XP18" s="11"/>
-      <c r="XQ18" s="11"/>
-      <c r="XR18" s="11"/>
-      <c r="XS18" s="11"/>
-      <c r="XT18" s="11"/>
-      <c r="XU18" s="11"/>
-      <c r="XV18" s="11"/>
-      <c r="XW18" s="11"/>
-      <c r="XX18" s="11"/>
-      <c r="XY18" s="11"/>
-      <c r="XZ18" s="11"/>
-      <c r="YA18" s="11"/>
-      <c r="YB18" s="11"/>
-      <c r="YC18" s="11"/>
-      <c r="YD18" s="11"/>
-      <c r="YE18" s="11"/>
-      <c r="YF18" s="11"/>
-      <c r="YG18" s="11"/>
-      <c r="YH18" s="11"/>
-      <c r="YI18" s="11"/>
-      <c r="YJ18" s="11"/>
-      <c r="YK18" s="11"/>
-      <c r="YL18" s="11"/>
-      <c r="YM18" s="11"/>
-      <c r="YN18" s="11"/>
-      <c r="YO18" s="11"/>
-      <c r="YP18" s="11"/>
-      <c r="YQ18" s="11"/>
-      <c r="YR18" s="11"/>
-      <c r="YS18" s="11"/>
-      <c r="YT18" s="11"/>
-      <c r="YU18" s="11"/>
-      <c r="YV18" s="11"/>
-      <c r="YW18" s="11"/>
-      <c r="YX18" s="11"/>
-      <c r="YY18" s="11"/>
-      <c r="YZ18" s="11"/>
-      <c r="ZA18" s="11"/>
-      <c r="ZB18" s="11"/>
-      <c r="ZC18" s="11"/>
-      <c r="ZD18" s="11"/>
-      <c r="ZE18" s="11"/>
-      <c r="ZF18" s="11"/>
-      <c r="ZG18" s="11"/>
-      <c r="ZH18" s="11"/>
-      <c r="ZI18" s="11"/>
-      <c r="ZJ18" s="11"/>
-      <c r="ZK18" s="11"/>
-      <c r="ZL18" s="11"/>
-      <c r="ZM18" s="11"/>
-      <c r="ZN18" s="11"/>
-      <c r="ZO18" s="11"/>
-      <c r="ZP18" s="11"/>
-      <c r="ZQ18" s="11"/>
-      <c r="ZR18" s="11"/>
-      <c r="ZS18" s="11"/>
-      <c r="ZT18" s="11"/>
-      <c r="ZU18" s="11"/>
-      <c r="ZV18" s="11"/>
-      <c r="ZW18" s="11"/>
-      <c r="ZX18" s="11"/>
-      <c r="ZY18" s="11"/>
-      <c r="ZZ18" s="11"/>
-      <c r="AAA18" s="11"/>
-      <c r="AAB18" s="11"/>
-      <c r="AAC18" s="11"/>
-      <c r="AAD18" s="11"/>
-      <c r="AAE18" s="11"/>
-      <c r="AAF18" s="11"/>
-      <c r="AAG18" s="11"/>
-      <c r="AAH18" s="11"/>
-      <c r="AAI18" s="11"/>
-      <c r="AAJ18" s="11"/>
-      <c r="AAK18" s="11"/>
-      <c r="AAL18" s="11"/>
-      <c r="AAM18" s="11"/>
-      <c r="AAN18" s="11"/>
-      <c r="AAO18" s="11"/>
-      <c r="AAP18" s="11"/>
-      <c r="AAQ18" s="11"/>
-      <c r="AAR18" s="11"/>
-      <c r="AAS18" s="11"/>
-      <c r="AAT18" s="11"/>
-      <c r="AAU18" s="11"/>
-      <c r="AAV18" s="11"/>
-      <c r="AAW18" s="11"/>
-      <c r="AAX18" s="11"/>
-      <c r="AAY18" s="11"/>
-      <c r="AAZ18" s="11"/>
-      <c r="ABA18" s="11"/>
-      <c r="ABB18" s="11"/>
-      <c r="ABC18" s="11"/>
-      <c r="ABD18" s="11"/>
-      <c r="ABE18" s="11"/>
-      <c r="ABF18" s="11"/>
-      <c r="ABG18" s="11"/>
-      <c r="ABH18" s="11"/>
-      <c r="ABI18" s="11"/>
-      <c r="ABJ18" s="11"/>
-      <c r="ABK18" s="11"/>
-      <c r="ABL18" s="11"/>
-      <c r="ABM18" s="11"/>
-      <c r="ABN18" s="11"/>
-      <c r="ABO18" s="11"/>
-      <c r="ABP18" s="11"/>
-      <c r="ABQ18" s="11"/>
-      <c r="ABR18" s="11"/>
-      <c r="ABS18" s="11"/>
-      <c r="ABT18" s="11"/>
-      <c r="ABU18" s="11"/>
-      <c r="ABV18" s="11"/>
-      <c r="ABW18" s="11"/>
-      <c r="ABX18" s="11"/>
-      <c r="ABY18" s="11"/>
-      <c r="ABZ18" s="11"/>
-      <c r="ACA18" s="11"/>
-      <c r="ACB18" s="11"/>
-      <c r="ACC18" s="11"/>
-      <c r="ACD18" s="11"/>
-      <c r="ACE18" s="11"/>
-      <c r="ACF18" s="11"/>
-      <c r="ACG18" s="11"/>
-      <c r="ACH18" s="11"/>
-      <c r="ACI18" s="11"/>
-      <c r="ACJ18" s="11"/>
-      <c r="ACK18" s="11"/>
-      <c r="ACL18" s="11"/>
-      <c r="ACM18" s="11"/>
-      <c r="ACN18" s="11"/>
-      <c r="ACO18" s="11"/>
-      <c r="ACP18" s="11"/>
-      <c r="ACQ18" s="11"/>
-      <c r="ACR18" s="11"/>
-      <c r="ACS18" s="11"/>
-      <c r="ACT18" s="11"/>
-      <c r="ACU18" s="11"/>
-      <c r="ACV18" s="11"/>
-      <c r="ACW18" s="11"/>
-      <c r="ACX18" s="11"/>
-      <c r="ACY18" s="11"/>
-      <c r="ACZ18" s="11"/>
-      <c r="ADA18" s="11"/>
-      <c r="ADB18" s="11"/>
-      <c r="ADC18" s="11"/>
-      <c r="ADD18" s="11"/>
-      <c r="ADE18" s="11"/>
-      <c r="ADF18" s="11"/>
-      <c r="ADG18" s="11"/>
-      <c r="ADH18" s="11"/>
-      <c r="ADI18" s="11"/>
-      <c r="ADJ18" s="11"/>
-      <c r="ADK18" s="11"/>
-      <c r="ADL18" s="11"/>
-      <c r="ADM18" s="11"/>
-      <c r="ADN18" s="11"/>
-      <c r="ADO18" s="11"/>
-      <c r="ADP18" s="11"/>
-      <c r="ADQ18" s="11"/>
-      <c r="ADR18" s="11"/>
-      <c r="ADS18" s="11"/>
-      <c r="ADT18" s="11"/>
-      <c r="ADU18" s="11"/>
-      <c r="ADV18" s="11"/>
-      <c r="ADW18" s="11"/>
-      <c r="ADX18" s="11"/>
-      <c r="ADY18" s="11"/>
-      <c r="ADZ18" s="11"/>
-      <c r="AEA18" s="11"/>
-      <c r="AEB18" s="11"/>
-      <c r="AEC18" s="11"/>
-      <c r="AED18" s="11"/>
-      <c r="AEE18" s="11"/>
-      <c r="AEF18" s="11"/>
-      <c r="AEG18" s="11"/>
-      <c r="AEH18" s="11"/>
-      <c r="AEI18" s="11"/>
-      <c r="AEJ18" s="11"/>
-      <c r="AEK18" s="11"/>
-      <c r="AEL18" s="11"/>
-      <c r="AEM18" s="11"/>
-      <c r="AEN18" s="11"/>
-      <c r="AEO18" s="11"/>
-      <c r="AEP18" s="11"/>
-      <c r="AEQ18" s="11"/>
-      <c r="AER18" s="11"/>
-      <c r="AES18" s="11"/>
-      <c r="AET18" s="11"/>
-      <c r="AEU18" s="11"/>
-      <c r="AEV18" s="11"/>
-      <c r="AEW18" s="11"/>
-      <c r="AEX18" s="11"/>
-      <c r="AEY18" s="11"/>
-      <c r="AEZ18" s="11"/>
-      <c r="AFA18" s="11"/>
-      <c r="AFB18" s="11"/>
-      <c r="AFC18" s="11"/>
-      <c r="AFD18" s="11"/>
-      <c r="AFE18" s="11"/>
-      <c r="AFF18" s="11"/>
-      <c r="AFG18" s="11"/>
-      <c r="AFH18" s="11"/>
-      <c r="AFI18" s="11"/>
-      <c r="AFJ18" s="11"/>
-      <c r="AFK18" s="11"/>
-      <c r="AFL18" s="11"/>
-      <c r="AFM18" s="11"/>
-      <c r="AFN18" s="11"/>
-      <c r="AFO18" s="11"/>
-      <c r="AFP18" s="11"/>
-      <c r="AFQ18" s="11"/>
-      <c r="AFR18" s="11"/>
-      <c r="AFS18" s="11"/>
-      <c r="AFT18" s="11"/>
-      <c r="AFU18" s="11"/>
-      <c r="AFV18" s="11"/>
-      <c r="AFW18" s="11"/>
-      <c r="AFX18" s="11"/>
-      <c r="AFY18" s="11"/>
-      <c r="AFZ18" s="11"/>
-      <c r="AGA18" s="11"/>
-      <c r="AGB18" s="11"/>
-      <c r="AGC18" s="11"/>
-      <c r="AGD18" s="11"/>
-      <c r="AGE18" s="11"/>
-      <c r="AGF18" s="11"/>
-      <c r="AGG18" s="11"/>
-      <c r="AGH18" s="11"/>
-      <c r="AGI18" s="11"/>
-      <c r="AGJ18" s="11"/>
-      <c r="AGK18" s="11"/>
-      <c r="AGL18" s="11"/>
-      <c r="AGM18" s="11"/>
-      <c r="AGN18" s="11"/>
-      <c r="AGO18" s="11"/>
-      <c r="AGP18" s="11"/>
-      <c r="AGQ18" s="11"/>
-      <c r="AGR18" s="11"/>
-      <c r="AGS18" s="11"/>
-      <c r="AGT18" s="11"/>
-      <c r="AGU18" s="11"/>
-      <c r="AGV18" s="11"/>
-      <c r="AGW18" s="11"/>
-      <c r="AGX18" s="11"/>
-      <c r="AGY18" s="11"/>
-      <c r="AGZ18" s="11"/>
-      <c r="AHA18" s="11"/>
-      <c r="AHB18" s="11"/>
-      <c r="AHC18" s="11"/>
-      <c r="AHD18" s="11"/>
-      <c r="AHE18" s="11"/>
-      <c r="AHF18" s="11"/>
-      <c r="AHG18" s="11"/>
-      <c r="AHH18" s="11"/>
-      <c r="AHI18" s="11"/>
-      <c r="AHJ18" s="11"/>
-      <c r="AHK18" s="11"/>
-      <c r="AHL18" s="11"/>
-      <c r="AHM18" s="11"/>
-      <c r="AHN18" s="11"/>
-      <c r="AHO18" s="11"/>
-      <c r="AHP18" s="11"/>
-      <c r="AHQ18" s="11"/>
-      <c r="AHR18" s="11"/>
-      <c r="AHS18" s="11"/>
-      <c r="AHT18" s="11"/>
-      <c r="AHU18" s="11"/>
-      <c r="AHV18" s="11"/>
-      <c r="AHW18" s="11"/>
-      <c r="AHX18" s="11"/>
-      <c r="AHY18" s="11"/>
-      <c r="AHZ18" s="11"/>
-      <c r="AIA18" s="11"/>
-      <c r="AIB18" s="11"/>
-      <c r="AIC18" s="11"/>
-      <c r="AID18" s="11"/>
-      <c r="AIE18" s="11"/>
-      <c r="AIF18" s="11"/>
-      <c r="AIG18" s="11"/>
-      <c r="AIH18" s="11"/>
-      <c r="AII18" s="11"/>
-      <c r="AIJ18" s="11"/>
-      <c r="AIK18" s="11"/>
-      <c r="AIL18" s="11"/>
-      <c r="AIM18" s="11"/>
-      <c r="AIN18" s="11"/>
-      <c r="AIO18" s="11"/>
-      <c r="AIP18" s="11"/>
-      <c r="AIQ18" s="11"/>
-      <c r="AIR18" s="11"/>
-      <c r="AIS18" s="11"/>
-      <c r="AIT18" s="11"/>
-      <c r="AIU18" s="11"/>
-      <c r="AIV18" s="11"/>
-      <c r="AIW18" s="11"/>
-      <c r="AIX18" s="11"/>
-      <c r="AIY18" s="11"/>
-      <c r="AIZ18" s="11"/>
-      <c r="AJA18" s="11"/>
-      <c r="AJB18" s="11"/>
-      <c r="AJC18" s="11"/>
-      <c r="AJD18" s="11"/>
-      <c r="AJE18" s="11"/>
-      <c r="AJF18" s="11"/>
-      <c r="AJG18" s="11"/>
-      <c r="AJH18" s="11"/>
-      <c r="AJI18" s="11"/>
-      <c r="AJJ18" s="11"/>
-      <c r="AJK18" s="11"/>
-      <c r="AJL18" s="11"/>
-      <c r="AJM18" s="11"/>
-      <c r="AJN18" s="11"/>
-      <c r="AJO18" s="11"/>
-      <c r="AJP18" s="11"/>
-      <c r="AJQ18" s="11"/>
-      <c r="AJR18" s="11"/>
-      <c r="AJS18" s="11"/>
-      <c r="AJT18" s="11"/>
-      <c r="AJU18" s="11"/>
-      <c r="AJV18" s="11"/>
-      <c r="AJW18" s="11"/>
-      <c r="AJX18" s="11"/>
-      <c r="AJY18" s="11"/>
-      <c r="AJZ18" s="11"/>
-      <c r="AKA18" s="11"/>
-      <c r="AKB18" s="11"/>
-      <c r="AKC18" s="11"/>
-      <c r="AKD18" s="11"/>
-      <c r="AKE18" s="11"/>
-      <c r="AKF18" s="11"/>
-      <c r="AKG18" s="11"/>
-      <c r="AKH18" s="11"/>
-      <c r="AKI18" s="11"/>
-      <c r="AKJ18" s="11"/>
-      <c r="AKK18" s="11"/>
-      <c r="AKL18" s="11"/>
-      <c r="AKM18" s="11"/>
-      <c r="AKN18" s="11"/>
-      <c r="AKO18" s="11"/>
-      <c r="AKP18" s="11"/>
-      <c r="AKQ18" s="11"/>
-      <c r="AKR18" s="11"/>
-      <c r="AKS18" s="11"/>
-      <c r="AKT18" s="11"/>
-      <c r="AKU18" s="11"/>
-      <c r="AKV18" s="11"/>
-      <c r="AKW18" s="11"/>
-      <c r="AKX18" s="11"/>
-      <c r="AKY18" s="11"/>
-      <c r="AKZ18" s="11"/>
-      <c r="ALA18" s="11"/>
-      <c r="ALB18" s="11"/>
-      <c r="ALC18" s="11"/>
-      <c r="ALD18" s="11"/>
-      <c r="ALE18" s="11"/>
-      <c r="ALF18" s="11"/>
-      <c r="ALG18" s="11"/>
-      <c r="ALH18" s="11"/>
-      <c r="ALI18" s="11"/>
-      <c r="ALJ18" s="11"/>
-      <c r="ALK18" s="11"/>
-      <c r="ALL18" s="11"/>
-      <c r="ALM18" s="11"/>
-      <c r="ALN18" s="11"/>
-      <c r="ALO18" s="11"/>
-      <c r="ALP18" s="11"/>
-      <c r="ALQ18" s="11"/>
-      <c r="ALR18" s="11"/>
-      <c r="ALS18" s="11"/>
-      <c r="ALT18" s="11"/>
-      <c r="ALU18" s="11"/>
-      <c r="ALV18" s="11"/>
-      <c r="ALW18" s="11"/>
-      <c r="ALX18" s="11"/>
-      <c r="ALY18" s="11"/>
-      <c r="ALZ18" s="11"/>
-      <c r="AMA18" s="11"/>
-      <c r="AMB18" s="11"/>
-      <c r="AMC18" s="11"/>
-      <c r="AMD18" s="11"/>
-      <c r="AME18" s="11"/>
-      <c r="AMF18" s="11"/>
-      <c r="AMG18" s="11"/>
-      <c r="AMH18" s="11"/>
-      <c r="AMI18" s="11"/>
-      <c r="AMJ18" s="11"/>
-      <c r="AMK18" s="11"/>
+      <c r="K18" s="15" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="19" spans="1:1025" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+    <row r="19" spans="1:1025" s="13" customFormat="1">
+      <c r="A19" s="10">
+        <v>3.15</v>
+      </c>
       <c r="B19" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>54</v>
@@ -16644,15 +13624,23 @@
         <v>69</v>
       </c>
       <c r="E19" s="12"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="G19" s="11"/>
       <c r="H19" s="11">
         <v>2</v>
       </c>
       <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="J19" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
@@ -17667,7 +14655,37 @@
       <c r="AMJ19" s="11"/>
       <c r="AMK19" s="11"/>
     </row>
-    <row r="37" spans="4:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1025">
+      <c r="A20" s="10">
+        <v>3.18</v>
+      </c>
+      <c r="B20" s="10">
+        <v>3</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="11">
+        <v>4</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="37" spans="4:4" ht="15" customHeight="1">
       <c r="D37" s="6" t="s">
         <v>60</v>
       </c>
@@ -17677,6 +14695,11 @@
     <sortCondition ref="K2:K17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>